<commit_message>
Completed and checked allocation plan execution by country
</commit_message>
<xml_diff>
--- a/SDBal/input_data.xlsx
+++ b/SDBal/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\SDBal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F015F320-8AC4-469B-9260-1956ADC0459D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64729F27-3A33-4E73-81BC-41585B30AF26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3432" yWindow="2856" windowWidth="15936" windowHeight="11556" tabRatio="723" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rank_sept" sheetId="21" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId11"/>
+    <pivotCache cacheId="7" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -59,7 +59,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fixed in month M-1</t>
@@ -74,7 +74,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -83,7 +83,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 To be updated in the middle/3rd week of month M (initial value from month M-1)</t>
@@ -122,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -131,7 +131,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -170,7 +170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -179,7 +179,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 To be fixed in month M</t>
@@ -387,7 +387,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -396,7 +396,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -411,7 +411,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -420,7 +420,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -445,7 +445,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -454,7 +454,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fixed</t>
@@ -469,7 +469,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -478,7 +478,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fixed</t>
@@ -493,7 +493,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -502,7 +502,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fixed</t>
@@ -517,7 +517,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -526,7 +526,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fixed</t>
@@ -565,7 +565,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -574,7 +574,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 To be fixed in month M</t>
@@ -613,7 +613,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -622,7 +622,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -661,7 +661,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -670,7 +670,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 To be fixed in month M</t>
@@ -878,7 +878,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -887,7 +887,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -902,7 +902,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -911,7 +911,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -923,7 +923,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="266">
   <si>
     <t>Lot Size (MT)</t>
   </si>
@@ -1721,6 +1721,9 @@
   <si>
     <t>Set by User</t>
   </si>
+  <si>
+    <t xml:space="preserve">Quantity to Trim: </t>
+  </si>
 </sst>
 </file>
 
@@ -1729,7 +1732,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14409]d\ mmmm\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1814,19 +1817,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2102,7 +2092,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="86">
+  <borders count="88">
     <border>
       <left/>
       <right/>
@@ -3197,6 +3187,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3204,11 +3224,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3328,20 +3348,20 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="56" xfId="4" applyBorder="1" applyAlignment="1">
@@ -3357,11 +3377,11 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3387,42 +3407,42 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="65" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="65" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="66" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="66" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="36" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="36" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="64" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="56" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="56" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3453,10 +3473,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3489,16 +3509,16 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3607,7 +3627,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3620,7 +3640,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="78" xfId="4" applyBorder="1" applyAlignment="1">
@@ -3647,7 +3667,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3666,134 +3686,35 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="26" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="19" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="83" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="83" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="68" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="45" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="45" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3807,13 +3728,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3822,10 +3737,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3855,31 +3770,25 @@
     <xf numFmtId="0" fontId="5" fillId="19" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="83" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="83" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3897,7 +3806,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="84" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="85" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="85" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3924,10 +3833,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3936,7 +3845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3945,7 +3854,7 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3963,28 +3872,138 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="86" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="87" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3998,11 +4017,165 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="258">
+  <dxfs count="245">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4066,251 +4239,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8472,7 +8400,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
@@ -10831,7 +10759,7 @@
       <c r="D86" s="18"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="54">
       <colorScale>
@@ -12023,7 +11951,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -13904,7 +13832,7 @@
       <c r="D86" s="18"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="54">
       <colorScale>
@@ -16630,7 +16558,7 @@
       <c r="K86"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="54">
       <colorScale>
@@ -20213,10 +20141,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="179" t="s">
+      <c r="D3" s="259" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="180"/>
+      <c r="E3" s="260"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -20329,11 +20257,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="214" t="s">
+      <c r="L14" s="235" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="214"/>
-      <c r="N14" s="214"/>
+      <c r="M14" s="235"/>
+      <c r="N14" s="235"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -20360,13 +20288,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="184" t="s">
+      <c r="F16" s="261" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="185" t="s">
+      <c r="G16" s="254" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="187" t="s">
+      <c r="H16" s="256" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -20390,9 +20318,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="184"/>
-      <c r="G17" s="186"/>
-      <c r="H17" s="188"/>
+      <c r="F17" s="261"/>
+      <c r="G17" s="255"/>
+      <c r="H17" s="244"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -20411,11 +20339,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="184"/>
-      <c r="G18" s="189" t="s">
+      <c r="F18" s="261"/>
+      <c r="G18" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="190" t="s">
+      <c r="H18" s="243" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -20438,9 +20366,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="184"/>
-      <c r="G19" s="186"/>
-      <c r="H19" s="188"/>
+      <c r="F19" s="261"/>
+      <c r="G19" s="255"/>
+      <c r="H19" s="244"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -20459,11 +20387,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="184"/>
-      <c r="G20" s="189" t="s">
+      <c r="F20" s="261"/>
+      <c r="G20" s="245" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="190" t="s">
+      <c r="H20" s="243" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -20487,9 +20415,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="184"/>
-      <c r="G21" s="186"/>
-      <c r="H21" s="188"/>
+      <c r="F21" s="261"/>
+      <c r="G21" s="255"/>
+      <c r="H21" s="244"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -20508,11 +20436,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="184"/>
-      <c r="G22" s="189" t="s">
+      <c r="F22" s="261"/>
+      <c r="G22" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="190" t="s">
+      <c r="H22" s="243" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -20536,9 +20464,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="184"/>
-      <c r="G23" s="191"/>
-      <c r="H23" s="192"/>
+      <c r="F23" s="261"/>
+      <c r="G23" s="246"/>
+      <c r="H23" s="247"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -20557,14 +20485,14 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="184"/>
+      <c r="F24" s="261"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
       <c r="J24" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="217">
+      <c r="K24" s="182">
         <v>2350</v>
       </c>
       <c r="L24" s="152">
@@ -20575,7 +20503,7 @@
         <f t="shared" ref="M24:N24" si="0">M16+M18+M20+M22</f>
         <v>2430</v>
       </c>
-      <c r="N24" s="219">
+      <c r="N24" s="184">
         <f t="shared" si="0"/>
         <v>2265</v>
       </c>
@@ -20587,10 +20515,10 @@
       <c r="J25" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="K25" s="216">
+      <c r="K25" s="181">
         <v>2200</v>
       </c>
-      <c r="L25" s="236">
+      <c r="L25" s="200">
         <f>shorttermplan2!K25</f>
         <v>2100</v>
       </c>
@@ -20602,18 +20530,18 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="177" t="s">
+      <c r="F26" s="257" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="177"/>
-      <c r="H26" s="177"/>
+      <c r="G26" s="257"/>
+      <c r="H26" s="257"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
       <c r="J26" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="K26" s="218">
+      <c r="K26" s="183">
         <v>2300</v>
       </c>
       <c r="L26" s="116">
@@ -20623,7 +20551,7 @@
         <f>IF(M24-M30&lt;=$D$10,M24-M30, $D$10)</f>
         <v>2400</v>
       </c>
-      <c r="N26" s="220">
+      <c r="N26" s="185">
         <f>IF(N24-N30&lt;=$D$10,N24-N30, $D$10)</f>
         <v>2190</v>
       </c>
@@ -20632,17 +20560,17 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="262" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="194"/>
+      <c r="H27" s="263"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
       <c r="J27" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="K27" s="212">
+      <c r="K27" s="179">
         <v>2650</v>
       </c>
       <c r="L27" s="3">
@@ -20653,14 +20581,14 @@
         <f t="shared" ref="M27:N27" si="1">L28+M26</f>
         <v>2805</v>
       </c>
-      <c r="N27" s="221">
+      <c r="N27" s="186">
         <f t="shared" si="1"/>
         <v>2565</v>
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="195"/>
-      <c r="H28" s="196"/>
+      <c r="G28" s="264"/>
+      <c r="H28" s="265"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -20679,34 +20607,34 @@
         <f t="shared" ref="M28:N28" si="2">M27-M24</f>
         <v>375</v>
       </c>
-      <c r="N28" s="222">
+      <c r="N28" s="187">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="195"/>
-      <c r="H29" s="196"/>
+      <c r="G29" s="264"/>
+      <c r="H29" s="265"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
       <c r="J29" s="117" t="s">
         <v>175</v>
       </c>
-      <c r="K29" s="223"/>
-      <c r="L29" s="246">
+      <c r="K29" s="188"/>
+      <c r="L29" s="209">
         <v>300</v>
       </c>
-      <c r="M29" s="245">
+      <c r="M29" s="208">
         <v>400</v>
       </c>
-      <c r="N29" s="244">
+      <c r="N29" s="207">
         <v>300</v>
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="195"/>
-      <c r="H30" s="196"/>
+      <c r="G30" s="264"/>
+      <c r="H30" s="265"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -20722,14 +20650,14 @@
         <f t="shared" ref="M30:N30" si="3">L28-M29</f>
         <v>5</v>
       </c>
-      <c r="N30" s="224">
+      <c r="N30" s="189">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="195"/>
-      <c r="H31" s="196"/>
+      <c r="G31" s="264"/>
+      <c r="H31" s="265"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -20745,14 +20673,14 @@
         <f>M26+M30</f>
         <v>2405</v>
       </c>
-      <c r="N31" s="224">
+      <c r="N31" s="189">
         <f>N26+N30</f>
         <v>2265</v>
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="197"/>
-      <c r="H32" s="198"/>
+      <c r="G32" s="266"/>
+      <c r="H32" s="267"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -20768,7 +20696,7 @@
         <f t="shared" ref="M32:N32" si="4">M31-M24</f>
         <v>-25</v>
       </c>
-      <c r="N32" s="225">
+      <c r="N32" s="190">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -20788,16 +20716,16 @@
         <f>IF(M24-M30&gt;$D$10, M24-M30 - $D$10, 0)</f>
         <v>25</v>
       </c>
-      <c r="N33" s="226">
+      <c r="N33" s="191">
         <f>IF(N24-N30&gt;$D$10, N24-N30 - $D$10, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="199" t="s">
+      <c r="G34" s="268" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="200"/>
+      <c r="H34" s="269"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -20819,8 +20747,8 @@
       </c>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G35" s="197"/>
-      <c r="H35" s="198"/>
+      <c r="G35" s="266"/>
+      <c r="H35" s="267"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -20921,11 +20849,11 @@
       </c>
     </row>
     <row r="40" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="177" t="s">
+      <c r="F40" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="177"/>
-      <c r="H40" s="178"/>
+      <c r="G40" s="257"/>
+      <c r="H40" s="258"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -20940,7 +20868,7 @@
         <f>M24</f>
         <v>2430</v>
       </c>
-      <c r="N40" s="227">
+      <c r="N40" s="192">
         <v>2265</v>
       </c>
     </row>
@@ -20956,17 +20884,17 @@
       <c r="M41" s="161" t="s">
         <v>126</v>
       </c>
-      <c r="N41" s="228">
+      <c r="N41" s="193">
         <f>N40-N24</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="177" t="s">
+      <c r="F42" s="257" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="177"/>
-      <c r="H42" s="178"/>
+      <c r="G42" s="257"/>
+      <c r="H42" s="258"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -20981,18 +20909,18 @@
         <f>M26</f>
         <v>2400</v>
       </c>
-      <c r="N42" s="229">
+      <c r="N42" s="194">
         <f>N26-N39+N41</f>
         <v>1695</v>
       </c>
     </row>
     <row r="43" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="201" t="s">
+      <c r="E43" s="238" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="201"/>
-      <c r="G43" s="201"/>
-      <c r="H43" s="201"/>
+      <c r="F43" s="238"/>
+      <c r="G43" s="238"/>
+      <c r="H43" s="238"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -21016,11 +20944,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="202" t="s">
+      <c r="L44" s="239" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="203"/>
-      <c r="N44" s="230" t="s">
+      <c r="M44" s="240"/>
+      <c r="N44" s="249" t="s">
         <v>77</v>
       </c>
     </row>
@@ -21028,16 +20956,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="202"/>
-      <c r="M45" s="203"/>
-      <c r="N45" s="215"/>
+      <c r="L45" s="239"/>
+      <c r="M45" s="240"/>
+      <c r="N45" s="250"/>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="204"/>
-      <c r="M46" s="205"/>
+      <c r="L46" s="241"/>
+      <c r="M46" s="242"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.3">
@@ -21111,10 +21039,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="181" t="s">
+      <c r="M55" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="182"/>
+      <c r="N55" s="252"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -21141,13 +21069,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="206" t="s">
+      <c r="F57" s="253" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="185" t="s">
+      <c r="G57" s="254" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="187" t="s">
+      <c r="H57" s="256" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -21171,9 +21099,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="206"/>
-      <c r="G58" s="186"/>
-      <c r="H58" s="188"/>
+      <c r="F58" s="253"/>
+      <c r="G58" s="255"/>
+      <c r="H58" s="244"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -21195,11 +21123,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="206"/>
-      <c r="G59" s="189" t="s">
+      <c r="F59" s="253"/>
+      <c r="G59" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="190" t="s">
+      <c r="H59" s="243" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -21223,9 +21151,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="206"/>
-      <c r="G60" s="186"/>
-      <c r="H60" s="188"/>
+      <c r="F60" s="253"/>
+      <c r="G60" s="255"/>
+      <c r="H60" s="244"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -21247,11 +21175,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="206"/>
-      <c r="G61" s="189" t="s">
+      <c r="F61" s="253"/>
+      <c r="G61" s="245" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="190" t="s">
+      <c r="H61" s="243" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -21275,9 +21203,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="206"/>
-      <c r="G62" s="186"/>
-      <c r="H62" s="188"/>
+      <c r="F62" s="253"/>
+      <c r="G62" s="255"/>
+      <c r="H62" s="244"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -21299,11 +21227,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="206"/>
-      <c r="G63" s="189" t="s">
+      <c r="F63" s="253"/>
+      <c r="G63" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="190" t="s">
+      <c r="H63" s="243" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -21327,9 +21255,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="206"/>
-      <c r="G64" s="191"/>
-      <c r="H64" s="192"/>
+      <c r="F64" s="253"/>
+      <c r="G64" s="246"/>
+      <c r="H64" s="247"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -21414,10 +21342,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="209" t="s">
+      <c r="G68" s="248" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="209"/>
+      <c r="H68" s="248"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -21439,8 +21367,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="209"/>
-      <c r="H69" s="209"/>
+      <c r="G69" s="248"/>
+      <c r="H69" s="248"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -21465,8 +21393,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="209"/>
-      <c r="H70" s="209"/>
+      <c r="G70" s="248"/>
+      <c r="H70" s="248"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -21488,10 +21416,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="207" t="s">
+      <c r="G71" s="236" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="208"/>
+      <c r="H71" s="237"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -21513,10 +21441,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="209" t="s">
+      <c r="G72" s="248" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="209"/>
+      <c r="H72" s="248"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -21538,8 +21466,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="209"/>
-      <c r="H73" s="209"/>
+      <c r="G73" s="248"/>
+      <c r="H73" s="248"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -21564,8 +21492,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="209"/>
-      <c r="H74" s="209"/>
+      <c r="G74" s="248"/>
+      <c r="H74" s="248"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -21585,10 +21513,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="207" t="s">
+      <c r="G75" s="236" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="208"/>
+      <c r="H75" s="237"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -21631,12 +21559,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="201" t="s">
+      <c r="E77" s="238" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="201"/>
-      <c r="G77" s="201"/>
-      <c r="H77" s="201"/>
+      <c r="F77" s="238"/>
+      <c r="G77" s="238"/>
+      <c r="H77" s="238"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -21655,18 +21583,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="202" t="s">
+      <c r="L78" s="239" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="203"/>
+      <c r="M78" s="240"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="202"/>
-      <c r="M79" s="203"/>
+      <c r="L79" s="239"/>
+      <c r="M79" s="240"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="204"/>
-      <c r="M80" s="205"/>
+      <c r="L80" s="241"/>
+      <c r="M80" s="242"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -21760,6 +21688,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="G27:H32"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F42:H42"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="G75:H75"/>
     <mergeCell ref="E77:H77"/>
@@ -21776,25 +21723,6 @@
     <mergeCell ref="M55:N55"/>
     <mergeCell ref="F57:F64"/>
     <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="G27:H32"/>
-    <mergeCell ref="G34:H35"/>
-    <mergeCell ref="F40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21859,10 +21787,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="179" t="s">
+      <c r="D3" s="259" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="180"/>
+      <c r="E3" s="260"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -21978,11 +21906,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="181" t="s">
+      <c r="L14" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="182"/>
-      <c r="N14" s="183"/>
+      <c r="M14" s="252"/>
+      <c r="N14" s="271"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -22009,13 +21937,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="184" t="s">
+      <c r="F16" s="261" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="185" t="s">
+      <c r="G16" s="254" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="187" t="s">
+      <c r="H16" s="256" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -22039,9 +21967,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="184"/>
-      <c r="G17" s="186"/>
-      <c r="H17" s="188"/>
+      <c r="F17" s="261"/>
+      <c r="G17" s="255"/>
+      <c r="H17" s="244"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -22049,7 +21977,7 @@
         <v>86</v>
       </c>
       <c r="K17" s="39"/>
-      <c r="L17" s="234" t="s">
+      <c r="L17" s="198" t="s">
         <v>126</v>
       </c>
       <c r="M17" s="167" t="s">
@@ -22060,11 +21988,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="184"/>
-      <c r="G18" s="189" t="s">
+      <c r="F18" s="261"/>
+      <c r="G18" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="190" t="s">
+      <c r="H18" s="243" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -22088,9 +22016,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="184"/>
-      <c r="G19" s="186"/>
-      <c r="H19" s="188"/>
+      <c r="F19" s="261"/>
+      <c r="G19" s="255"/>
+      <c r="H19" s="244"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -22098,7 +22026,7 @@
         <v>87</v>
       </c>
       <c r="K19" s="40"/>
-      <c r="L19" s="234" t="s">
+      <c r="L19" s="198" t="s">
         <v>126</v>
       </c>
       <c r="M19" s="168" t="s">
@@ -22109,11 +22037,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="184"/>
-      <c r="G20" s="189" t="s">
+      <c r="F20" s="261"/>
+      <c r="G20" s="245" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="190" t="s">
+      <c r="H20" s="243" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -22137,17 +22065,17 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="184"/>
-      <c r="G21" s="186"/>
-      <c r="H21" s="188"/>
+      <c r="F21" s="261"/>
+      <c r="G21" s="255"/>
+      <c r="H21" s="244"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
       <c r="J21" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="231"/>
-      <c r="L21" s="234" t="s">
+      <c r="K21" s="195"/>
+      <c r="L21" s="198" t="s">
         <v>126</v>
       </c>
       <c r="M21" s="168" t="s">
@@ -22158,11 +22086,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="184"/>
-      <c r="G22" s="189" t="s">
+      <c r="F22" s="261"/>
+      <c r="G22" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="190" t="s">
+      <c r="H22" s="243" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -22171,7 +22099,7 @@
       <c r="J22" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="K22" s="232"/>
+      <c r="K22" s="196"/>
       <c r="L22" s="153">
         <f>shorttermplan1!L22</f>
         <v>890</v>
@@ -22186,17 +22114,17 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="184"/>
-      <c r="G23" s="191"/>
-      <c r="H23" s="192"/>
+      <c r="F23" s="261"/>
+      <c r="G23" s="246"/>
+      <c r="H23" s="247"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
       <c r="J23" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="233"/>
-      <c r="L23" s="235" t="s">
+      <c r="K23" s="197"/>
+      <c r="L23" s="199" t="s">
         <v>126</v>
       </c>
       <c r="M23" s="169" t="s">
@@ -22207,14 +22135,14 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="184"/>
+      <c r="F24" s="261"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
       <c r="J24" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="213">
+      <c r="K24" s="180">
         <f>shorttermplan1!L24</f>
         <v>2395</v>
       </c>
@@ -22225,7 +22153,7 @@
       <c r="M24" s="152">
         <v>3000</v>
       </c>
-      <c r="N24" s="219">
+      <c r="N24" s="184">
         <v>2285</v>
       </c>
     </row>
@@ -22239,7 +22167,7 @@
       <c r="K25" s="175">
         <v>2100</v>
       </c>
-      <c r="L25" s="238">
+      <c r="L25" s="201">
         <v>2200</v>
       </c>
       <c r="M25" s="170" t="s">
@@ -22250,18 +22178,18 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="177" t="s">
+      <c r="F26" s="257" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="177"/>
-      <c r="H26" s="177"/>
+      <c r="G26" s="257"/>
+      <c r="H26" s="257"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
       <c r="J26" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="K26" s="211">
+      <c r="K26" s="178">
         <f>shorttermplan1!L26</f>
         <v>2350</v>
       </c>
@@ -22273,7 +22201,7 @@
         <f>IF(M24-M30&lt;=$D$10,M24-M30, $D$10)</f>
         <v>2400</v>
       </c>
-      <c r="N26" s="220">
+      <c r="N26" s="185">
         <f>IF(N24-N30&lt;=$D$10,N24-N30, $D$10)</f>
         <v>2400</v>
       </c>
@@ -22282,17 +22210,17 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="262" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="194"/>
+      <c r="H27" s="263"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J27" s="239" t="s">
+      <c r="J27" s="202" t="s">
         <v>142</v>
       </c>
-      <c r="K27" s="212">
+      <c r="K27" s="179">
         <f>shorttermplan1!L27</f>
         <v>2800</v>
       </c>
@@ -22304,18 +22232,18 @@
         <f t="shared" ref="M27:N27" si="0">L28+M26</f>
         <v>3070</v>
       </c>
-      <c r="N27" s="221">
+      <c r="N27" s="186">
         <f t="shared" si="0"/>
         <v>2470</v>
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="195"/>
-      <c r="H28" s="196"/>
+      <c r="G28" s="264"/>
+      <c r="H28" s="265"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J28" s="240" t="s">
+      <c r="J28" s="203" t="s">
         <v>143</v>
       </c>
       <c r="K28" s="120">
@@ -22330,38 +22258,38 @@
         <f t="shared" ref="M28:N28" si="1">M27-M24</f>
         <v>70</v>
       </c>
-      <c r="N28" s="222">
+      <c r="N28" s="187">
         <f t="shared" si="1"/>
         <v>185</v>
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="195"/>
-      <c r="H29" s="196"/>
+      <c r="G29" s="264"/>
+      <c r="H29" s="265"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="J29" s="240" t="s">
+      <c r="J29" s="203" t="s">
         <v>175</v>
       </c>
-      <c r="K29" s="223"/>
-      <c r="L29" s="243">
+      <c r="K29" s="188"/>
+      <c r="L29" s="206">
         <v>300</v>
       </c>
-      <c r="M29" s="245">
+      <c r="M29" s="208">
         <v>350</v>
       </c>
-      <c r="N29" s="244">
+      <c r="N29" s="207">
         <v>200</v>
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="195"/>
-      <c r="H30" s="196"/>
+      <c r="G30" s="264"/>
+      <c r="H30" s="265"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="J30" s="240" t="s">
+      <c r="J30" s="203" t="s">
         <v>144</v>
       </c>
       <c r="K30" s="119"/>
@@ -22373,18 +22301,18 @@
         <f t="shared" ref="M30:N30" si="2">L28-M29</f>
         <v>320</v>
       </c>
-      <c r="N30" s="224">
+      <c r="N30" s="189">
         <f t="shared" si="2"/>
         <v>-130</v>
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="195"/>
-      <c r="H31" s="196"/>
+      <c r="G31" s="264"/>
+      <c r="H31" s="265"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="J31" s="241" t="s">
+      <c r="J31" s="204" t="s">
         <v>145</v>
       </c>
       <c r="K31" s="119"/>
@@ -22396,14 +22324,14 @@
         <f>M26+M30</f>
         <v>2720</v>
       </c>
-      <c r="N31" s="224">
+      <c r="N31" s="189">
         <f>N26+N30</f>
         <v>2270</v>
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="197"/>
-      <c r="H32" s="198"/>
+      <c r="G32" s="266"/>
+      <c r="H32" s="267"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -22419,7 +22347,7 @@
         <f t="shared" ref="M32:N32" si="3">M31-M24</f>
         <v>-280</v>
       </c>
-      <c r="N32" s="225">
+      <c r="N32" s="190">
         <f t="shared" si="3"/>
         <v>-15</v>
       </c>
@@ -22439,16 +22367,16 @@
         <f>IF(M24-M30&gt;$D$10, M24-M30 - $D$10, 0)</f>
         <v>280</v>
       </c>
-      <c r="N33" s="226">
+      <c r="N33" s="191">
         <f>IF(N24-N30&gt;$D$10, N24-N30 - $D$10, 0)</f>
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="5:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="199" t="s">
+      <c r="G34" s="268" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="200"/>
+      <c r="H34" s="269"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -22470,8 +22398,8 @@
       </c>
     </row>
     <row r="35" spans="5:21" x14ac:dyDescent="0.3">
-      <c r="G35" s="197"/>
-      <c r="H35" s="198"/>
+      <c r="G35" s="266"/>
+      <c r="H35" s="267"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -22516,7 +22444,7 @@
       <c r="I37" s="127" t="s">
         <v>141</v>
       </c>
-      <c r="J37" s="242" t="s">
+      <c r="J37" s="205" t="s">
         <v>150</v>
       </c>
       <c r="K37" s="132"/>
@@ -22572,11 +22500,11 @@
       </c>
     </row>
     <row r="40" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="177" t="s">
+      <c r="F40" s="257" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="177"/>
-      <c r="H40" s="178"/>
+      <c r="G40" s="257"/>
+      <c r="H40" s="258"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -22591,7 +22519,7 @@
         <f>M24</f>
         <v>3000</v>
       </c>
-      <c r="N40" s="227">
+      <c r="N40" s="192">
         <v>2265</v>
       </c>
     </row>
@@ -22607,17 +22535,17 @@
       <c r="M41" s="161" t="s">
         <v>126</v>
       </c>
-      <c r="N41" s="228">
+      <c r="N41" s="193">
         <f>N40-N24</f>
         <v>-20</v>
       </c>
     </row>
     <row r="42" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="177" t="s">
+      <c r="F42" s="257" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="177"/>
-      <c r="H42" s="178"/>
+      <c r="G42" s="257"/>
+      <c r="H42" s="258"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -22632,18 +22560,18 @@
         <f>M26</f>
         <v>2400</v>
       </c>
-      <c r="N42" s="229">
+      <c r="N42" s="194">
         <f>N26-N39+N41</f>
         <v>2000</v>
       </c>
     </row>
     <row r="43" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="201" t="s">
+      <c r="E43" s="238" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="201"/>
-      <c r="G43" s="201"/>
-      <c r="H43" s="201"/>
+      <c r="F43" s="238"/>
+      <c r="G43" s="238"/>
+      <c r="H43" s="238"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -22665,11 +22593,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="202" t="s">
+      <c r="L44" s="239" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="203"/>
-      <c r="N44" s="237" t="s">
+      <c r="M44" s="240"/>
+      <c r="N44" s="270" t="s">
         <v>77</v>
       </c>
     </row>
@@ -22677,16 +22605,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="202"/>
-      <c r="M45" s="203"/>
-      <c r="N45" s="215"/>
+      <c r="L45" s="239"/>
+      <c r="M45" s="240"/>
+      <c r="N45" s="250"/>
     </row>
     <row r="46" spans="5:21" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="204"/>
-      <c r="M46" s="205"/>
+      <c r="L46" s="241"/>
+      <c r="M46" s="242"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:21" x14ac:dyDescent="0.3">
@@ -22768,10 +22696,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="181" t="s">
+      <c r="M55" s="251" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="182"/>
+      <c r="N55" s="252"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -22798,13 +22726,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="206" t="s">
+      <c r="F57" s="253" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="185" t="s">
+      <c r="G57" s="254" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="187" t="s">
+      <c r="H57" s="256" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -22828,9 +22756,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="206"/>
-      <c r="G58" s="186"/>
-      <c r="H58" s="188"/>
+      <c r="F58" s="253"/>
+      <c r="G58" s="255"/>
+      <c r="H58" s="244"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -22852,11 +22780,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="206"/>
-      <c r="G59" s="189" t="s">
+      <c r="F59" s="253"/>
+      <c r="G59" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="190" t="s">
+      <c r="H59" s="243" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -22880,9 +22808,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="206"/>
-      <c r="G60" s="186"/>
-      <c r="H60" s="188"/>
+      <c r="F60" s="253"/>
+      <c r="G60" s="255"/>
+      <c r="H60" s="244"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -22904,11 +22832,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="206"/>
-      <c r="G61" s="189" t="s">
+      <c r="F61" s="253"/>
+      <c r="G61" s="245" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="190" t="s">
+      <c r="H61" s="243" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -22932,9 +22860,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="206"/>
-      <c r="G62" s="186"/>
-      <c r="H62" s="188"/>
+      <c r="F62" s="253"/>
+      <c r="G62" s="255"/>
+      <c r="H62" s="244"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -22956,11 +22884,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="206"/>
-      <c r="G63" s="189" t="s">
+      <c r="F63" s="253"/>
+      <c r="G63" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="190" t="s">
+      <c r="H63" s="243" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -22984,9 +22912,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="206"/>
-      <c r="G64" s="191"/>
-      <c r="H64" s="192"/>
+      <c r="F64" s="253"/>
+      <c r="G64" s="246"/>
+      <c r="H64" s="247"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -23071,10 +22999,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="209" t="s">
+      <c r="G68" s="248" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="209"/>
+      <c r="H68" s="248"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -23096,8 +23024,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="209"/>
-      <c r="H69" s="209"/>
+      <c r="G69" s="248"/>
+      <c r="H69" s="248"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -23122,8 +23050,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="209"/>
-      <c r="H70" s="209"/>
+      <c r="G70" s="248"/>
+      <c r="H70" s="248"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -23145,10 +23073,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="207" t="s">
+      <c r="G71" s="236" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="208"/>
+      <c r="H71" s="237"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -23170,10 +23098,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="209" t="s">
+      <c r="G72" s="248" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="209"/>
+      <c r="H72" s="248"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -23195,8 +23123,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="209"/>
-      <c r="H73" s="209"/>
+      <c r="G73" s="248"/>
+      <c r="H73" s="248"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -23221,8 +23149,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="209"/>
-      <c r="H74" s="209"/>
+      <c r="G74" s="248"/>
+      <c r="H74" s="248"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -23242,10 +23170,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="207" t="s">
+      <c r="G75" s="236" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="208"/>
+      <c r="H75" s="237"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -23288,12 +23216,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="201" t="s">
+      <c r="E77" s="238" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="201"/>
-      <c r="G77" s="201"/>
-      <c r="H77" s="201"/>
+      <c r="F77" s="238"/>
+      <c r="G77" s="238"/>
+      <c r="H77" s="238"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -23312,18 +23240,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="202" t="s">
+      <c r="L78" s="239" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="203"/>
+      <c r="M78" s="240"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="202"/>
-      <c r="M79" s="203"/>
+      <c r="L79" s="239"/>
+      <c r="M79" s="240"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="204"/>
-      <c r="M80" s="205"/>
+      <c r="L80" s="241"/>
+      <c r="M80" s="242"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -23411,6 +23339,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="N44:N45"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="L44:M46"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
     <mergeCell ref="L78:M80"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="F26:H26"/>
@@ -23427,25 +23374,6 @@
     <mergeCell ref="G57:G58"/>
     <mergeCell ref="H57:H58"/>
     <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="N44:N45"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="L44:M46"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="L14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23493,7 +23421,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="263" t="s">
+      <c r="A3" s="226" t="s">
         <v>258</v>
       </c>
       <c r="B3" t="s">
@@ -23501,346 +23429,346 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="227" t="s">
         <v>189</v>
       </c>
-      <c r="B4" s="267">
+      <c r="B4" s="230">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="265" t="s">
+      <c r="A5" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="267">
+      <c r="B5" s="230">
         <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="266" t="s">
+      <c r="A6" s="229" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="267">
+      <c r="B6" s="230">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="266" t="s">
+      <c r="A7" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="267">
+      <c r="B7" s="230">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="266" t="s">
+      <c r="A8" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="267">
+      <c r="B8" s="230">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="266" t="s">
+      <c r="A9" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B9" s="267">
+      <c r="B9" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="264" t="s">
+      <c r="A10" s="227" t="s">
         <v>190</v>
       </c>
-      <c r="B10" s="267">
+      <c r="B10" s="230">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="265" t="s">
+      <c r="A11" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="267">
+      <c r="B11" s="230">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="266" t="s">
+      <c r="A12" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="267">
+      <c r="B12" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="266" t="s">
+      <c r="A13" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="267">
+      <c r="B13" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="266" t="s">
+      <c r="A14" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B14" s="267">
+      <c r="B14" s="230">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="264" t="s">
+      <c r="A15" s="227" t="s">
         <v>194</v>
       </c>
-      <c r="B15" s="267">
+      <c r="B15" s="230">
         <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="265" t="s">
+      <c r="A16" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="267">
+      <c r="B16" s="230">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="266" t="s">
+      <c r="A17" s="229" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="267">
+      <c r="B17" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="266" t="s">
+      <c r="A18" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="267">
+      <c r="B18" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="266" t="s">
+      <c r="A19" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="267">
+      <c r="B19" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="266" t="s">
+      <c r="A20" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B20" s="267">
+      <c r="B20" s="230">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="264" t="s">
+      <c r="A21" s="227" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="267">
+      <c r="B21" s="230">
         <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="265" t="s">
+      <c r="A22" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="267">
+      <c r="B22" s="230">
         <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="266" t="s">
+      <c r="A23" s="229" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="267">
+      <c r="B23" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="266" t="s">
+      <c r="A24" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="267">
+      <c r="B24" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="266" t="s">
+      <c r="A25" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="267">
+      <c r="B25" s="230">
         <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="266" t="s">
+      <c r="A26" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B26" s="267">
+      <c r="B26" s="230">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="264" t="s">
+      <c r="A27" s="227" t="s">
         <v>196</v>
       </c>
-      <c r="B27" s="267">
+      <c r="B27" s="230">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="265" t="s">
+      <c r="A28" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="267">
+      <c r="B28" s="230">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="266" t="s">
+      <c r="A29" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="267">
+      <c r="B29" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="266" t="s">
+      <c r="A30" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="267">
+      <c r="B30" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="266" t="s">
+      <c r="A31" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B31" s="267">
+      <c r="B31" s="230">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="264" t="s">
+      <c r="A32" s="227" t="s">
         <v>199</v>
       </c>
-      <c r="B32" s="267">
+      <c r="B32" s="230">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="265" t="s">
+      <c r="A33" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="267">
+      <c r="B33" s="230">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="266" t="s">
+      <c r="A34" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="267">
+      <c r="B34" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="266" t="s">
+      <c r="A35" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B35" s="267">
+      <c r="B35" s="230">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="264" t="s">
+      <c r="A36" s="227" t="s">
         <v>200</v>
       </c>
-      <c r="B36" s="267">
+      <c r="B36" s="230">
         <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="265" t="s">
+      <c r="A37" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="267">
+      <c r="B37" s="230">
         <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="266" t="s">
+      <c r="A38" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="267">
+      <c r="B38" s="230">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="266" t="s">
+      <c r="A39" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="267">
+      <c r="B39" s="230">
         <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="266" t="s">
+      <c r="A40" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B40" s="267">
+      <c r="B40" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="264" t="s">
+      <c r="A41" s="227" t="s">
         <v>201</v>
       </c>
-      <c r="B41" s="267">
+      <c r="B41" s="230">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="265" t="s">
+      <c r="A42" s="228" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="267">
+      <c r="B42" s="230">
         <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="266" t="s">
+      <c r="A43" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="267">
+      <c r="B43" s="230">
         <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="266" t="s">
+      <c r="A44" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="267">
+      <c r="B44" s="230">
         <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="266" t="s">
+      <c r="A45" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="B45" s="267">
+      <c r="B45" s="230">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="264" t="s">
+      <c r="A46" s="227" t="s">
         <v>259</v>
       </c>
-      <c r="B46" s="267">
+      <c r="B46" s="230">
         <v>785</v>
       </c>
     </row>
@@ -23853,8 +23781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA26EA1-65D7-4B0C-A5C0-83D8CE19816C}">
   <dimension ref="C2:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23869,7 +23797,7 @@
     <col min="9" max="9" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
@@ -23883,7 +23811,7 @@
       <c r="D2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="262" t="s">
+      <c r="E2" s="225" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="17" t="s">
@@ -23936,17 +23864,17 @@
       <c r="J3" s="23">
         <v>400</v>
       </c>
-      <c r="N3" s="210" t="s">
+      <c r="N3" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="269" t="s">
+      <c r="O3" s="231" t="s">
         <v>263</v>
       </c>
-      <c r="P3" s="248"/>
-      <c r="Q3" s="210" t="s">
+      <c r="P3" s="211"/>
+      <c r="Q3" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="269" t="s">
+      <c r="R3" s="231" t="s">
         <v>263</v>
       </c>
     </row>
@@ -23975,17 +23903,17 @@
       <c r="J4" s="27">
         <v>20</v>
       </c>
-      <c r="N4" s="270" t="s">
+      <c r="N4" s="232" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="271">
+      <c r="O4" s="275">
         <v>10</v>
       </c>
-      <c r="P4" s="248"/>
-      <c r="Q4" s="270" t="s">
+      <c r="P4" s="211"/>
+      <c r="Q4" s="232" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="271">
+      <c r="R4" s="275">
         <v>10</v>
       </c>
     </row>
@@ -24014,17 +23942,17 @@
       <c r="J5" s="27">
         <v>10</v>
       </c>
-      <c r="N5" s="272" t="s">
+      <c r="N5" s="233" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="273">
+      <c r="O5" s="275">
         <v>50</v>
       </c>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="272" t="s">
+      <c r="P5" s="211"/>
+      <c r="Q5" s="233" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="273">
+      <c r="R5" s="275">
         <v>25</v>
       </c>
     </row>
@@ -24053,17 +23981,17 @@
       <c r="J6" s="27">
         <v>200</v>
       </c>
-      <c r="N6" s="272" t="s">
+      <c r="N6" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="273">
+      <c r="O6" s="275">
         <v>70</v>
       </c>
-      <c r="P6" s="248"/>
-      <c r="Q6" s="272" t="s">
+      <c r="P6" s="211"/>
+      <c r="Q6" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="R6" s="273">
+      <c r="R6" s="275">
         <v>50</v>
       </c>
     </row>
@@ -24092,17 +24020,17 @@
       <c r="J7" s="27">
         <v>20</v>
       </c>
-      <c r="N7" s="274" t="s">
+      <c r="N7" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="O7" s="275">
+      <c r="O7" s="276">
         <v>80</v>
       </c>
-      <c r="P7" s="248"/>
-      <c r="Q7" s="274" t="s">
+      <c r="P7" s="211"/>
+      <c r="Q7" s="234" t="s">
         <v>241</v>
       </c>
-      <c r="R7" s="275">
+      <c r="R7" s="276">
         <v>70</v>
       </c>
     </row>
@@ -24131,14 +24059,14 @@
       <c r="J8" s="27">
         <v>25</v>
       </c>
-      <c r="N8" s="268" t="s">
+      <c r="N8" s="272" t="s">
         <v>264</v>
       </c>
-      <c r="O8" s="268"/>
-      <c r="Q8" s="268" t="s">
+      <c r="O8" s="272"/>
+      <c r="Q8" s="272" t="s">
         <v>264</v>
       </c>
-      <c r="R8" s="268"/>
+      <c r="R8" s="272"/>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C9" s="24" t="s">
@@ -24220,6 +24148,12 @@
       <c r="J11" s="27">
         <v>20</v>
       </c>
+      <c r="M11" s="273" t="s">
+        <v>265</v>
+      </c>
+      <c r="N11" s="274">
+        <v>300</v>
+      </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C12" s="24" t="s">
@@ -24793,7 +24727,7 @@
       <c r="I31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="261">
+      <c r="J31" s="224">
         <v>0</v>
       </c>
     </row>
@@ -24819,7 +24753,7 @@
       <c r="I32" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="J32" s="261">
+      <c r="J32" s="224">
         <v>50</v>
       </c>
     </row>
@@ -25736,7 +25670,7 @@
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="Q8:R8"/>
   </mergeCells>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="54">
       <colorScale>
@@ -26425,11 +26359,11 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="247" customWidth="1"/>
-    <col min="4" max="5" width="19" style="247" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="248" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="248" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="247" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="210" customWidth="1"/>
+    <col min="4" max="5" width="19" style="210" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="211" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="211" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="210" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
@@ -26438,589 +26372,589 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="249" t="s">
+      <c r="C4" s="212" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="249" t="s">
+      <c r="D4" s="212" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="249" t="s">
+      <c r="E4" s="212" t="s">
         <v>209</v>
       </c>
-      <c r="F4" s="250" t="s">
+      <c r="F4" s="213" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="250" t="s">
+      <c r="G4" s="213" t="s">
         <v>247</v>
       </c>
-      <c r="H4" s="249" t="s">
+      <c r="H4" s="212" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="255" t="s">
+      <c r="C5" s="218" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="255" t="s">
+      <c r="D5" s="218" t="s">
         <v>189</v>
       </c>
-      <c r="E5" s="255" t="s">
+      <c r="E5" s="218" t="s">
         <v>242</v>
       </c>
-      <c r="F5" s="256" t="s">
+      <c r="F5" s="219" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="256"/>
+      <c r="H5" s="219"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="255"/>
-      <c r="D6" s="255"/>
-      <c r="E6" s="255" t="s">
+      <c r="C6" s="218"/>
+      <c r="D6" s="218"/>
+      <c r="E6" s="218" t="s">
         <v>243</v>
       </c>
-      <c r="F6" s="256" t="s">
+      <c r="F6" s="219" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="256"/>
+      <c r="H6" s="219"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="255"/>
-      <c r="D7" s="255"/>
-      <c r="E7" s="255" t="s">
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218" t="s">
         <v>244</v>
       </c>
-      <c r="F7" s="256" t="s">
+      <c r="F7" s="219" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="256"/>
+      <c r="H7" s="219"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255" t="s">
+      <c r="C8" s="218"/>
+      <c r="D8" s="218"/>
+      <c r="E8" s="218" t="s">
         <v>245</v>
       </c>
-      <c r="F8" s="256" t="s">
+      <c r="F8" s="219" t="s">
         <v>240</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="256"/>
+      <c r="H8" s="219"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="255"/>
-      <c r="D9" s="255"/>
-      <c r="E9" s="255" t="s">
+      <c r="C9" s="218"/>
+      <c r="D9" s="218"/>
+      <c r="E9" s="218" t="s">
         <v>248</v>
       </c>
-      <c r="F9" s="256" t="s">
+      <c r="F9" s="219" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="256"/>
+      <c r="H9" s="219"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="255"/>
-      <c r="D10" s="255"/>
-      <c r="E10" s="255" t="s">
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218" t="s">
         <v>249</v>
       </c>
-      <c r="F10" s="256" t="s">
+      <c r="F10" s="219" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="256"/>
+      <c r="H10" s="219"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="255"/>
-      <c r="D11" s="255"/>
-      <c r="E11" s="255" t="s">
+      <c r="C11" s="218"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218" t="s">
         <v>250</v>
       </c>
-      <c r="F11" s="256" t="s">
+      <c r="F11" s="219" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="256"/>
+      <c r="H11" s="219"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="255"/>
-      <c r="D12" s="255"/>
-      <c r="E12" s="255" t="s">
+      <c r="C12" s="218"/>
+      <c r="D12" s="218"/>
+      <c r="E12" s="218" t="s">
         <v>251</v>
       </c>
-      <c r="F12" s="256" t="s">
+      <c r="F12" s="219" t="s">
         <v>240</v>
       </c>
       <c r="G12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="256"/>
+      <c r="H12" s="219"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="255"/>
-      <c r="D13" s="255"/>
-      <c r="E13" s="257" t="s">
+      <c r="C13" s="218"/>
+      <c r="D13" s="218"/>
+      <c r="E13" s="220" t="s">
         <v>246</v>
       </c>
-      <c r="F13" s="256" t="s">
+      <c r="F13" s="219" t="s">
         <v>241</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="256">
+      <c r="H13" s="219">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="258" t="s">
+      <c r="C14" s="221" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="258" t="s">
+      <c r="D14" s="221" t="s">
         <v>189</v>
       </c>
-      <c r="E14" s="258" t="s">
+      <c r="E14" s="221" t="s">
         <v>225</v>
       </c>
-      <c r="F14" s="259" t="s">
+      <c r="F14" s="222" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="259"/>
-      <c r="H14" s="259"/>
+      <c r="G14" s="222"/>
+      <c r="H14" s="222"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="258"/>
-      <c r="D15" s="258"/>
-      <c r="E15" s="258" t="s">
+      <c r="C15" s="221"/>
+      <c r="D15" s="221"/>
+      <c r="E15" s="221" t="s">
         <v>226</v>
       </c>
-      <c r="F15" s="259" t="s">
+      <c r="F15" s="222" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="259"/>
-      <c r="H15" s="259"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="222"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="258"/>
-      <c r="D16" s="258"/>
-      <c r="E16" s="258" t="s">
+      <c r="C16" s="221"/>
+      <c r="D16" s="221"/>
+      <c r="E16" s="221" t="s">
         <v>227</v>
       </c>
-      <c r="F16" s="259" t="s">
+      <c r="F16" s="222" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="259"/>
-      <c r="H16" s="259"/>
+      <c r="G16" s="222"/>
+      <c r="H16" s="222"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C17" s="258"/>
-      <c r="D17" s="258"/>
-      <c r="E17" s="258" t="s">
+      <c r="C17" s="221"/>
+      <c r="D17" s="221"/>
+      <c r="E17" s="221" t="s">
         <v>228</v>
       </c>
-      <c r="F17" s="259" t="s">
+      <c r="F17" s="222" t="s">
         <v>240</v>
       </c>
-      <c r="G17" s="259"/>
-      <c r="H17" s="259"/>
+      <c r="G17" s="222"/>
+      <c r="H17" s="222"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C18" s="258"/>
-      <c r="D18" s="258"/>
-      <c r="E18" s="258" t="s">
+      <c r="C18" s="221"/>
+      <c r="D18" s="221"/>
+      <c r="E18" s="221" t="s">
         <v>252</v>
       </c>
-      <c r="F18" s="259" t="s">
+      <c r="F18" s="222" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="259"/>
-      <c r="H18" s="259"/>
+      <c r="G18" s="222"/>
+      <c r="H18" s="222"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="258"/>
-      <c r="D19" s="258"/>
-      <c r="E19" s="258" t="s">
+      <c r="C19" s="221"/>
+      <c r="D19" s="221"/>
+      <c r="E19" s="221" t="s">
         <v>253</v>
       </c>
-      <c r="F19" s="259" t="s">
+      <c r="F19" s="222" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="259"/>
-      <c r="H19" s="259"/>
+      <c r="G19" s="222"/>
+      <c r="H19" s="222"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C20" s="258"/>
-      <c r="D20" s="258"/>
-      <c r="E20" s="258" t="s">
+      <c r="C20" s="221"/>
+      <c r="D20" s="221"/>
+      <c r="E20" s="221" t="s">
         <v>254</v>
       </c>
-      <c r="F20" s="259" t="s">
+      <c r="F20" s="222" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="259"/>
-      <c r="H20" s="259"/>
+      <c r="G20" s="222"/>
+      <c r="H20" s="222"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C21" s="258"/>
-      <c r="D21" s="258"/>
-      <c r="E21" s="258" t="s">
+      <c r="C21" s="221"/>
+      <c r="D21" s="221"/>
+      <c r="E21" s="221" t="s">
         <v>255</v>
       </c>
-      <c r="F21" s="259" t="s">
+      <c r="F21" s="222" t="s">
         <v>240</v>
       </c>
-      <c r="G21" s="259"/>
-      <c r="H21" s="259"/>
+      <c r="G21" s="222"/>
+      <c r="H21" s="222"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="258"/>
-      <c r="D22" s="258"/>
-      <c r="E22" s="260" t="s">
+      <c r="C22" s="221"/>
+      <c r="D22" s="221"/>
+      <c r="E22" s="223" t="s">
         <v>211</v>
       </c>
-      <c r="F22" s="259" t="s">
+      <c r="F22" s="222" t="s">
         <v>241</v>
       </c>
-      <c r="G22" s="259"/>
-      <c r="H22" s="259">
+      <c r="G22" s="222"/>
+      <c r="H22" s="222">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C23" s="247" t="s">
+      <c r="C23" s="210" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="247" t="s">
+      <c r="D23" s="210" t="s">
         <v>189</v>
       </c>
-      <c r="E23" s="247" t="s">
+      <c r="E23" s="210" t="s">
         <v>221</v>
       </c>
-      <c r="F23" s="248" t="s">
+      <c r="F23" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="248"/>
+      <c r="H23" s="211"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="247" t="s">
+      <c r="E24" s="210" t="s">
         <v>222</v>
       </c>
-      <c r="F24" s="248" t="s">
+      <c r="F24" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="248"/>
+      <c r="H24" s="211"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E25" s="247" t="s">
+      <c r="E25" s="210" t="s">
         <v>223</v>
       </c>
-      <c r="F25" s="248" t="s">
+      <c r="F25" s="211" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="248"/>
+      <c r="H25" s="211"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E26" s="247" t="s">
+      <c r="E26" s="210" t="s">
         <v>224</v>
       </c>
-      <c r="F26" s="248" t="s">
+      <c r="F26" s="211" t="s">
         <v>240</v>
       </c>
-      <c r="H26" s="248"/>
+      <c r="H26" s="211"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E27" s="254" t="s">
+      <c r="E27" s="217" t="s">
         <v>210</v>
       </c>
-      <c r="F27" s="248" t="s">
+      <c r="F27" s="211" t="s">
         <v>241</v>
       </c>
-      <c r="H27" s="248">
+      <c r="H27" s="211">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C28" s="251" t="s">
+      <c r="C28" s="214" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="251" t="s">
+      <c r="D28" s="214" t="s">
         <v>194</v>
       </c>
-      <c r="E28" s="251" t="s">
+      <c r="E28" s="214" t="s">
         <v>217</v>
       </c>
-      <c r="F28" s="252" t="s">
+      <c r="F28" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="252"/>
-      <c r="H28" s="252"/>
+      <c r="G28" s="215"/>
+      <c r="H28" s="215"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C29" s="251"/>
-      <c r="D29" s="251"/>
-      <c r="E29" s="251" t="s">
+      <c r="C29" s="214"/>
+      <c r="D29" s="214"/>
+      <c r="E29" s="214" t="s">
         <v>218</v>
       </c>
-      <c r="F29" s="252" t="s">
+      <c r="F29" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="252"/>
-      <c r="H29" s="252"/>
+      <c r="G29" s="215"/>
+      <c r="H29" s="215"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="251"/>
-      <c r="D30" s="251"/>
-      <c r="E30" s="251" t="s">
+      <c r="C30" s="214"/>
+      <c r="D30" s="214"/>
+      <c r="E30" s="214" t="s">
         <v>219</v>
       </c>
-      <c r="F30" s="252" t="s">
+      <c r="F30" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="252"/>
-      <c r="H30" s="252"/>
+      <c r="G30" s="215"/>
+      <c r="H30" s="215"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C31" s="251"/>
-      <c r="D31" s="251"/>
-      <c r="E31" s="251" t="s">
+      <c r="C31" s="214"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214" t="s">
         <v>220</v>
       </c>
-      <c r="F31" s="252" t="s">
+      <c r="F31" s="215" t="s">
         <v>240</v>
       </c>
-      <c r="G31" s="252"/>
-      <c r="H31" s="252"/>
+      <c r="G31" s="215"/>
+      <c r="H31" s="215"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C32" s="251"/>
-      <c r="D32" s="251"/>
-      <c r="E32" s="253" t="s">
+      <c r="C32" s="214"/>
+      <c r="D32" s="214"/>
+      <c r="E32" s="216" t="s">
         <v>212</v>
       </c>
-      <c r="F32" s="252" t="s">
+      <c r="F32" s="215" t="s">
         <v>241</v>
       </c>
-      <c r="G32" s="252"/>
-      <c r="H32" s="252">
+      <c r="G32" s="215"/>
+      <c r="H32" s="215">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C33" s="247" t="s">
+      <c r="C33" s="210" t="s">
         <v>184</v>
       </c>
-      <c r="D33" s="247" t="s">
+      <c r="D33" s="210" t="s">
         <v>195</v>
       </c>
-      <c r="E33" s="247" t="s">
+      <c r="E33" s="210" t="s">
         <v>229</v>
       </c>
-      <c r="F33" s="248" t="s">
+      <c r="F33" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="248"/>
+      <c r="H33" s="211"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E34" s="247" t="s">
+      <c r="E34" s="210" t="s">
         <v>230</v>
       </c>
-      <c r="F34" s="248" t="s">
+      <c r="F34" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="248"/>
+      <c r="H34" s="211"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E35" s="247" t="s">
+      <c r="E35" s="210" t="s">
         <v>213</v>
       </c>
-      <c r="F35" s="248" t="s">
+      <c r="F35" s="211" t="s">
         <v>241</v>
       </c>
-      <c r="H35" s="248"/>
+      <c r="H35" s="211"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C36" s="251" t="s">
+      <c r="C36" s="214" t="s">
         <v>185</v>
       </c>
-      <c r="D36" s="251" t="s">
+      <c r="D36" s="214" t="s">
         <v>196</v>
       </c>
-      <c r="E36" s="251" t="s">
+      <c r="E36" s="214" t="s">
         <v>214</v>
       </c>
-      <c r="F36" s="252" t="s">
+      <c r="F36" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="252"/>
-      <c r="H36" s="252"/>
+      <c r="G36" s="215"/>
+      <c r="H36" s="215"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C37" s="251"/>
-      <c r="D37" s="251"/>
-      <c r="E37" s="251" t="s">
+      <c r="C37" s="214"/>
+      <c r="D37" s="214"/>
+      <c r="E37" s="214" t="s">
         <v>215</v>
       </c>
-      <c r="F37" s="252" t="s">
+      <c r="F37" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="252"/>
-      <c r="H37" s="252"/>
+      <c r="G37" s="215"/>
+      <c r="H37" s="215"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C38" s="251"/>
-      <c r="D38" s="251"/>
-      <c r="E38" s="253" t="s">
+      <c r="C38" s="214"/>
+      <c r="D38" s="214"/>
+      <c r="E38" s="216" t="s">
         <v>216</v>
       </c>
-      <c r="F38" s="252" t="s">
+      <c r="F38" s="215" t="s">
         <v>241</v>
       </c>
-      <c r="G38" s="252"/>
-      <c r="H38" s="252">
+      <c r="G38" s="215"/>
+      <c r="H38" s="215">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C39" s="247" t="s">
+      <c r="C39" s="210" t="s">
         <v>186</v>
       </c>
-      <c r="D39" s="247" t="s">
+      <c r="D39" s="210" t="s">
         <v>199</v>
       </c>
-      <c r="E39" s="247" t="s">
+      <c r="E39" s="210" t="s">
         <v>231</v>
       </c>
-      <c r="F39" s="248" t="s">
+      <c r="F39" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="248"/>
+      <c r="H39" s="211"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E40" s="247" t="s">
+      <c r="E40" s="210" t="s">
         <v>232</v>
       </c>
-      <c r="F40" s="248" t="s">
+      <c r="F40" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="H40" s="248"/>
+      <c r="H40" s="211"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E41" s="247" t="s">
+      <c r="E41" s="210" t="s">
         <v>233</v>
       </c>
-      <c r="F41" s="248" t="s">
+      <c r="F41" s="211" t="s">
         <v>241</v>
       </c>
-      <c r="H41" s="248"/>
+      <c r="H41" s="211"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C42" s="251" t="s">
+      <c r="C42" s="214" t="s">
         <v>187</v>
       </c>
-      <c r="D42" s="251" t="s">
+      <c r="D42" s="214" t="s">
         <v>200</v>
       </c>
-      <c r="E42" s="251" t="s">
+      <c r="E42" s="214" t="s">
         <v>234</v>
       </c>
-      <c r="F42" s="252" t="s">
+      <c r="F42" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="252"/>
-      <c r="H42" s="252"/>
+      <c r="G42" s="215"/>
+      <c r="H42" s="215"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C43" s="251"/>
-      <c r="D43" s="251"/>
-      <c r="E43" s="251" t="s">
+      <c r="C43" s="214"/>
+      <c r="D43" s="214"/>
+      <c r="E43" s="214" t="s">
         <v>235</v>
       </c>
-      <c r="F43" s="252" t="s">
+      <c r="F43" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="G43" s="252"/>
-      <c r="H43" s="252"/>
+      <c r="G43" s="215"/>
+      <c r="H43" s="215"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C44" s="251"/>
-      <c r="D44" s="251"/>
-      <c r="E44" s="253" t="s">
+      <c r="C44" s="214"/>
+      <c r="D44" s="214"/>
+      <c r="E44" s="216" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="252" t="s">
+      <c r="F44" s="215" t="s">
         <v>241</v>
       </c>
-      <c r="G44" s="252"/>
-      <c r="H44" s="252">
+      <c r="G44" s="215"/>
+      <c r="H44" s="215">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C45" s="247" t="s">
+      <c r="C45" s="210" t="s">
         <v>188</v>
       </c>
-      <c r="D45" s="247" t="s">
+      <c r="D45" s="210" t="s">
         <v>204</v>
       </c>
-      <c r="E45" s="247" t="s">
+      <c r="E45" s="210" t="s">
         <v>237</v>
       </c>
-      <c r="F45" s="248" t="s">
+      <c r="F45" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="248"/>
+      <c r="H45" s="211"/>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E46" s="247" t="s">
+      <c r="E46" s="210" t="s">
         <v>238</v>
       </c>
-      <c r="F46" s="248" t="s">
+      <c r="F46" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="H46" s="248"/>
+      <c r="H46" s="211"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E47" s="254" t="s">
+      <c r="E47" s="217" t="s">
         <v>239</v>
       </c>
-      <c r="F47" s="248" t="s">
+      <c r="F47" s="211" t="s">
         <v>241</v>
       </c>
-      <c r="H47" s="248">
+      <c r="H47" s="211">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H48" s="248"/>
+      <c r="H48" s="211"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H49" s="248"/>
+      <c r="H49" s="211"/>
     </row>
     <row r="50" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H50" s="248"/>
+      <c r="H50" s="211"/>
     </row>
     <row r="51" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H51" s="248"/>
+      <c r="H51" s="211"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
complete allocation execution by customer
</commit_message>
<xml_diff>
--- a/SDBal/input_data.xlsx
+++ b/SDBal/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\SDBal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64729F27-3A33-4E73-81BC-41585B30AF26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30E0F65-2BBF-460D-9617-068398A8F698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rank_sept" sheetId="21" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -923,7 +923,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="268">
   <si>
     <t>Lot Size (MT)</t>
   </si>
@@ -1713,9 +1713,6 @@
     <t>Reduction criteria:</t>
   </si>
   <si>
-    <t>Company level</t>
-  </si>
-  <si>
     <t>perctg cut</t>
   </si>
   <si>
@@ -1723,6 +1720,15 @@
   </si>
   <si>
     <t xml:space="preserve">Quantity to Trim: </t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Customer level</t>
+  </si>
+  <si>
+    <t>cust_perctg cut</t>
   </si>
 </sst>
 </file>
@@ -3884,6 +3890,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="86" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="87" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3956,15 +3970,6 @@
     <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3989,6 +3994,15 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3997,14 +4011,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="86" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="87" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -8400,7 +8406,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
@@ -11596,8 +11602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCC809B-A99B-4A75-BBB5-8AF73C253AC5}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11841,7 +11847,7 @@
         <v>196</v>
       </c>
       <c r="P16" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -20141,10 +20147,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="259" t="s">
+      <c r="D3" s="271" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="260"/>
+      <c r="E3" s="272"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -20257,11 +20263,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="235" t="s">
+      <c r="L14" s="239" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="235"/>
-      <c r="N14" s="235"/>
+      <c r="M14" s="239"/>
+      <c r="N14" s="239"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -20288,13 +20294,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="261" t="s">
+      <c r="F16" s="273" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="254" t="s">
+      <c r="G16" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="256" t="s">
+      <c r="H16" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -20318,9 +20324,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="261"/>
-      <c r="G17" s="255"/>
-      <c r="H17" s="244"/>
+      <c r="F17" s="273"/>
+      <c r="G17" s="259"/>
+      <c r="H17" s="248"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -20339,11 +20345,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="261"/>
-      <c r="G18" s="245" t="s">
+      <c r="F18" s="273"/>
+      <c r="G18" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="243" t="s">
+      <c r="H18" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -20366,9 +20372,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="261"/>
-      <c r="G19" s="255"/>
-      <c r="H19" s="244"/>
+      <c r="F19" s="273"/>
+      <c r="G19" s="259"/>
+      <c r="H19" s="248"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -20387,11 +20393,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="261"/>
-      <c r="G20" s="245" t="s">
+      <c r="F20" s="273"/>
+      <c r="G20" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="243" t="s">
+      <c r="H20" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -20415,9 +20421,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="261"/>
-      <c r="G21" s="255"/>
-      <c r="H21" s="244"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="259"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -20436,11 +20442,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="261"/>
-      <c r="G22" s="245" t="s">
+      <c r="F22" s="273"/>
+      <c r="G22" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="243" t="s">
+      <c r="H22" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -20464,9 +20470,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="261"/>
-      <c r="G23" s="246"/>
-      <c r="H23" s="247"/>
+      <c r="F23" s="273"/>
+      <c r="G23" s="250"/>
+      <c r="H23" s="251"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -20485,7 +20491,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="261"/>
+      <c r="F24" s="273"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -20530,11 +20536,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="257" t="s">
+      <c r="F26" s="261" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="257"/>
-      <c r="H26" s="257"/>
+      <c r="G26" s="261"/>
+      <c r="H26" s="261"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -20560,10 +20566,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="262" t="s">
+      <c r="G27" s="263" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="263"/>
+      <c r="H27" s="264"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -20587,8 +20593,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="264"/>
-      <c r="H28" s="265"/>
+      <c r="G28" s="265"/>
+      <c r="H28" s="266"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -20613,8 +20619,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="264"/>
-      <c r="H29" s="265"/>
+      <c r="G29" s="265"/>
+      <c r="H29" s="266"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -20633,8 +20639,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="264"/>
-      <c r="H30" s="265"/>
+      <c r="G30" s="265"/>
+      <c r="H30" s="266"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -20656,8 +20662,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="264"/>
-      <c r="H31" s="265"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="266"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -20679,8 +20685,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="266"/>
-      <c r="H32" s="267"/>
+      <c r="G32" s="267"/>
+      <c r="H32" s="268"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -20722,10 +20728,10 @@
       </c>
     </row>
     <row r="34" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="268" t="s">
+      <c r="G34" s="269" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="269"/>
+      <c r="H34" s="270"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -20747,8 +20753,8 @@
       </c>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G35" s="266"/>
-      <c r="H35" s="267"/>
+      <c r="G35" s="267"/>
+      <c r="H35" s="268"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -20849,11 +20855,11 @@
       </c>
     </row>
     <row r="40" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="257" t="s">
+      <c r="F40" s="261" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="257"/>
-      <c r="H40" s="258"/>
+      <c r="G40" s="261"/>
+      <c r="H40" s="262"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -20890,11 +20896,11 @@
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="257" t="s">
+      <c r="F42" s="261" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="257"/>
-      <c r="H42" s="258"/>
+      <c r="G42" s="261"/>
+      <c r="H42" s="262"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -20915,12 +20921,12 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="238" t="s">
+      <c r="E43" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="238"/>
-      <c r="G43" s="238"/>
-      <c r="H43" s="238"/>
+      <c r="F43" s="242"/>
+      <c r="G43" s="242"/>
+      <c r="H43" s="242"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -20944,11 +20950,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="239" t="s">
+      <c r="L44" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="240"/>
-      <c r="N44" s="249" t="s">
+      <c r="M44" s="244"/>
+      <c r="N44" s="253" t="s">
         <v>77</v>
       </c>
     </row>
@@ -20956,16 +20962,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="239"/>
-      <c r="M45" s="240"/>
-      <c r="N45" s="250"/>
+      <c r="L45" s="243"/>
+      <c r="M45" s="244"/>
+      <c r="N45" s="254"/>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="241"/>
-      <c r="M46" s="242"/>
+      <c r="L46" s="245"/>
+      <c r="M46" s="246"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.3">
@@ -21039,10 +21045,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="251" t="s">
+      <c r="M55" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="252"/>
+      <c r="N55" s="256"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -21069,13 +21075,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="253" t="s">
+      <c r="F57" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="254" t="s">
+      <c r="G57" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="256" t="s">
+      <c r="H57" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -21099,9 +21105,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="253"/>
-      <c r="G58" s="255"/>
-      <c r="H58" s="244"/>
+      <c r="F58" s="257"/>
+      <c r="G58" s="259"/>
+      <c r="H58" s="248"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -21123,11 +21129,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="253"/>
-      <c r="G59" s="245" t="s">
+      <c r="F59" s="257"/>
+      <c r="G59" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="243" t="s">
+      <c r="H59" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -21151,9 +21157,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="253"/>
-      <c r="G60" s="255"/>
-      <c r="H60" s="244"/>
+      <c r="F60" s="257"/>
+      <c r="G60" s="259"/>
+      <c r="H60" s="248"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -21175,11 +21181,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="253"/>
-      <c r="G61" s="245" t="s">
+      <c r="F61" s="257"/>
+      <c r="G61" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="243" t="s">
+      <c r="H61" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -21203,9 +21209,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="253"/>
-      <c r="G62" s="255"/>
-      <c r="H62" s="244"/>
+      <c r="F62" s="257"/>
+      <c r="G62" s="259"/>
+      <c r="H62" s="248"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -21227,11 +21233,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="253"/>
-      <c r="G63" s="245" t="s">
+      <c r="F63" s="257"/>
+      <c r="G63" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="243" t="s">
+      <c r="H63" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -21255,9 +21261,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="253"/>
-      <c r="G64" s="246"/>
-      <c r="H64" s="247"/>
+      <c r="F64" s="257"/>
+      <c r="G64" s="250"/>
+      <c r="H64" s="251"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -21342,10 +21348,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="248" t="s">
+      <c r="G68" s="252" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="248"/>
+      <c r="H68" s="252"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -21367,8 +21373,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="248"/>
-      <c r="H69" s="248"/>
+      <c r="G69" s="252"/>
+      <c r="H69" s="252"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -21393,8 +21399,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="248"/>
-      <c r="H70" s="248"/>
+      <c r="G70" s="252"/>
+      <c r="H70" s="252"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -21416,10 +21422,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="236" t="s">
+      <c r="G71" s="240" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="237"/>
+      <c r="H71" s="241"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -21441,10 +21447,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="248" t="s">
+      <c r="G72" s="252" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="248"/>
+      <c r="H72" s="252"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -21466,8 +21472,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="248"/>
-      <c r="H73" s="248"/>
+      <c r="G73" s="252"/>
+      <c r="H73" s="252"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -21492,8 +21498,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="248"/>
-      <c r="H74" s="248"/>
+      <c r="G74" s="252"/>
+      <c r="H74" s="252"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -21513,10 +21519,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="236" t="s">
+      <c r="G75" s="240" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="237"/>
+      <c r="H75" s="241"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -21559,12 +21565,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="238" t="s">
+      <c r="E77" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="238"/>
-      <c r="G77" s="238"/>
-      <c r="H77" s="238"/>
+      <c r="F77" s="242"/>
+      <c r="G77" s="242"/>
+      <c r="H77" s="242"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -21583,18 +21589,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="239" t="s">
+      <c r="L78" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="240"/>
+      <c r="M78" s="244"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="239"/>
-      <c r="M79" s="240"/>
+      <c r="L79" s="243"/>
+      <c r="M79" s="244"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="241"/>
-      <c r="M80" s="242"/>
+      <c r="L80" s="245"/>
+      <c r="M80" s="246"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -21787,10 +21793,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="259" t="s">
+      <c r="D3" s="271" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="260"/>
+      <c r="E3" s="272"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -21906,11 +21912,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="251" t="s">
+      <c r="L14" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="252"/>
-      <c r="N14" s="271"/>
+      <c r="M14" s="256"/>
+      <c r="N14" s="275"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -21937,13 +21943,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="261" t="s">
+      <c r="F16" s="273" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="254" t="s">
+      <c r="G16" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="256" t="s">
+      <c r="H16" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -21967,9 +21973,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="261"/>
-      <c r="G17" s="255"/>
-      <c r="H17" s="244"/>
+      <c r="F17" s="273"/>
+      <c r="G17" s="259"/>
+      <c r="H17" s="248"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -21988,11 +21994,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="261"/>
-      <c r="G18" s="245" t="s">
+      <c r="F18" s="273"/>
+      <c r="G18" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="243" t="s">
+      <c r="H18" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -22016,9 +22022,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="261"/>
-      <c r="G19" s="255"/>
-      <c r="H19" s="244"/>
+      <c r="F19" s="273"/>
+      <c r="G19" s="259"/>
+      <c r="H19" s="248"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -22037,11 +22043,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="261"/>
-      <c r="G20" s="245" t="s">
+      <c r="F20" s="273"/>
+      <c r="G20" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="243" t="s">
+      <c r="H20" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -22065,9 +22071,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="261"/>
-      <c r="G21" s="255"/>
-      <c r="H21" s="244"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="259"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -22086,11 +22092,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="261"/>
-      <c r="G22" s="245" t="s">
+      <c r="F22" s="273"/>
+      <c r="G22" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="243" t="s">
+      <c r="H22" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -22114,9 +22120,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="261"/>
-      <c r="G23" s="246"/>
-      <c r="H23" s="247"/>
+      <c r="F23" s="273"/>
+      <c r="G23" s="250"/>
+      <c r="H23" s="251"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -22135,7 +22141,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="261"/>
+      <c r="F24" s="273"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -22178,11 +22184,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="257" t="s">
+      <c r="F26" s="261" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="257"/>
-      <c r="H26" s="257"/>
+      <c r="G26" s="261"/>
+      <c r="H26" s="261"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -22210,10 +22216,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="262" t="s">
+      <c r="G27" s="263" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="263"/>
+      <c r="H27" s="264"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -22238,8 +22244,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="264"/>
-      <c r="H28" s="265"/>
+      <c r="G28" s="265"/>
+      <c r="H28" s="266"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -22264,8 +22270,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="264"/>
-      <c r="H29" s="265"/>
+      <c r="G29" s="265"/>
+      <c r="H29" s="266"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -22284,8 +22290,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="264"/>
-      <c r="H30" s="265"/>
+      <c r="G30" s="265"/>
+      <c r="H30" s="266"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -22307,8 +22313,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="264"/>
-      <c r="H31" s="265"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="266"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -22330,8 +22336,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="266"/>
-      <c r="H32" s="267"/>
+      <c r="G32" s="267"/>
+      <c r="H32" s="268"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -22373,10 +22379,10 @@
       </c>
     </row>
     <row r="34" spans="5:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="268" t="s">
+      <c r="G34" s="269" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="269"/>
+      <c r="H34" s="270"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -22398,8 +22404,8 @@
       </c>
     </row>
     <row r="35" spans="5:21" x14ac:dyDescent="0.3">
-      <c r="G35" s="266"/>
-      <c r="H35" s="267"/>
+      <c r="G35" s="267"/>
+      <c r="H35" s="268"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -22500,11 +22506,11 @@
       </c>
     </row>
     <row r="40" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="257" t="s">
+      <c r="F40" s="261" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="257"/>
-      <c r="H40" s="258"/>
+      <c r="G40" s="261"/>
+      <c r="H40" s="262"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -22541,11 +22547,11 @@
       </c>
     </row>
     <row r="42" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="257" t="s">
+      <c r="F42" s="261" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="257"/>
-      <c r="H42" s="258"/>
+      <c r="G42" s="261"/>
+      <c r="H42" s="262"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -22566,12 +22572,12 @@
       </c>
     </row>
     <row r="43" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="238" t="s">
+      <c r="E43" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="238"/>
-      <c r="G43" s="238"/>
-      <c r="H43" s="238"/>
+      <c r="F43" s="242"/>
+      <c r="G43" s="242"/>
+      <c r="H43" s="242"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -22593,11 +22599,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="239" t="s">
+      <c r="L44" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="240"/>
-      <c r="N44" s="270" t="s">
+      <c r="M44" s="244"/>
+      <c r="N44" s="274" t="s">
         <v>77</v>
       </c>
     </row>
@@ -22605,16 +22611,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="239"/>
-      <c r="M45" s="240"/>
-      <c r="N45" s="250"/>
+      <c r="L45" s="243"/>
+      <c r="M45" s="244"/>
+      <c r="N45" s="254"/>
     </row>
     <row r="46" spans="5:21" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="241"/>
-      <c r="M46" s="242"/>
+      <c r="L46" s="245"/>
+      <c r="M46" s="246"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:21" x14ac:dyDescent="0.3">
@@ -22696,10 +22702,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="251" t="s">
+      <c r="M55" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="252"/>
+      <c r="N55" s="256"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -22726,13 +22732,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="253" t="s">
+      <c r="F57" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="254" t="s">
+      <c r="G57" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="256" t="s">
+      <c r="H57" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -22756,9 +22762,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="253"/>
-      <c r="G58" s="255"/>
-      <c r="H58" s="244"/>
+      <c r="F58" s="257"/>
+      <c r="G58" s="259"/>
+      <c r="H58" s="248"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -22780,11 +22786,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="253"/>
-      <c r="G59" s="245" t="s">
+      <c r="F59" s="257"/>
+      <c r="G59" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="243" t="s">
+      <c r="H59" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -22808,9 +22814,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="253"/>
-      <c r="G60" s="255"/>
-      <c r="H60" s="244"/>
+      <c r="F60" s="257"/>
+      <c r="G60" s="259"/>
+      <c r="H60" s="248"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -22832,11 +22838,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="253"/>
-      <c r="G61" s="245" t="s">
+      <c r="F61" s="257"/>
+      <c r="G61" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="243" t="s">
+      <c r="H61" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -22860,9 +22866,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="253"/>
-      <c r="G62" s="255"/>
-      <c r="H62" s="244"/>
+      <c r="F62" s="257"/>
+      <c r="G62" s="259"/>
+      <c r="H62" s="248"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -22884,11 +22890,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="253"/>
-      <c r="G63" s="245" t="s">
+      <c r="F63" s="257"/>
+      <c r="G63" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="243" t="s">
+      <c r="H63" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -22912,9 +22918,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="253"/>
-      <c r="G64" s="246"/>
-      <c r="H64" s="247"/>
+      <c r="F64" s="257"/>
+      <c r="G64" s="250"/>
+      <c r="H64" s="251"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -22999,10 +23005,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="248" t="s">
+      <c r="G68" s="252" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="248"/>
+      <c r="H68" s="252"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -23024,8 +23030,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="248"/>
-      <c r="H69" s="248"/>
+      <c r="G69" s="252"/>
+      <c r="H69" s="252"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -23050,8 +23056,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="248"/>
-      <c r="H70" s="248"/>
+      <c r="G70" s="252"/>
+      <c r="H70" s="252"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -23073,10 +23079,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="236" t="s">
+      <c r="G71" s="240" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="237"/>
+      <c r="H71" s="241"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -23098,10 +23104,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="248" t="s">
+      <c r="G72" s="252" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="248"/>
+      <c r="H72" s="252"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -23123,8 +23129,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="248"/>
-      <c r="H73" s="248"/>
+      <c r="G73" s="252"/>
+      <c r="H73" s="252"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -23149,8 +23155,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="248"/>
-      <c r="H74" s="248"/>
+      <c r="G74" s="252"/>
+      <c r="H74" s="252"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -23170,10 +23176,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="236" t="s">
+      <c r="G75" s="240" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="237"/>
+      <c r="H75" s="241"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -23216,12 +23222,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="238" t="s">
+      <c r="E77" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="238"/>
-      <c r="G77" s="238"/>
-      <c r="H77" s="238"/>
+      <c r="F77" s="242"/>
+      <c r="G77" s="242"/>
+      <c r="H77" s="242"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -23240,18 +23246,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="239" t="s">
+      <c r="L78" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="240"/>
+      <c r="M78" s="244"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="239"/>
-      <c r="M79" s="240"/>
+      <c r="L79" s="243"/>
+      <c r="M79" s="244"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="241"/>
-      <c r="M80" s="242"/>
+      <c r="L80" s="245"/>
+      <c r="M80" s="246"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -23779,10 +23785,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA26EA1-65D7-4B0C-A5C0-83D8CE19816C}">
-  <dimension ref="C2:R86"/>
+  <dimension ref="C2:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23799,12 +23805,12 @@
     <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
     <col min="17" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
@@ -23839,7 +23845,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="20" t="s">
         <v>17</v>
       </c>
@@ -23868,17 +23874,17 @@
         <v>20</v>
       </c>
       <c r="O3" s="231" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P3" s="211"/>
       <c r="Q3" s="177" t="s">
         <v>22</v>
       </c>
       <c r="R3" s="231" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C4" s="24" t="s">
         <v>17</v>
       </c>
@@ -23906,18 +23912,18 @@
       <c r="N4" s="232" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="275">
+      <c r="O4" s="237">
         <v>10</v>
       </c>
       <c r="P4" s="211"/>
       <c r="Q4" s="232" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="275">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="R4" s="237">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C5" s="24" t="s">
         <v>17</v>
       </c>
@@ -23945,18 +23951,18 @@
       <c r="N5" s="233" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="275">
+      <c r="O5" s="237">
         <v>50</v>
       </c>
       <c r="P5" s="211"/>
       <c r="Q5" s="233" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="275">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="R5" s="237">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C6" s="24" t="s">
         <v>17</v>
       </c>
@@ -23984,18 +23990,18 @@
       <c r="N6" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="275">
+      <c r="O6" s="237">
         <v>70</v>
       </c>
       <c r="P6" s="211"/>
       <c r="Q6" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="R6" s="275">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R6" s="237">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="24" t="s">
         <v>17</v>
       </c>
@@ -24023,18 +24029,18 @@
       <c r="N7" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="O7" s="276">
+      <c r="O7" s="238">
         <v>80</v>
       </c>
       <c r="P7" s="211"/>
       <c r="Q7" s="234" t="s">
         <v>241</v>
       </c>
-      <c r="R7" s="276">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="R7" s="238">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C8" s="24" t="s">
         <v>17</v>
       </c>
@@ -24059,16 +24065,16 @@
       <c r="J8" s="27">
         <v>25</v>
       </c>
-      <c r="N8" s="272" t="s">
-        <v>264</v>
-      </c>
-      <c r="O8" s="272"/>
-      <c r="Q8" s="272" t="s">
-        <v>264</v>
-      </c>
-      <c r="R8" s="272"/>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="N8" s="276" t="s">
+        <v>263</v>
+      </c>
+      <c r="O8" s="276"/>
+      <c r="Q8" s="276" t="s">
+        <v>263</v>
+      </c>
+      <c r="R8" s="276"/>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C9" s="24" t="s">
         <v>17</v>
       </c>
@@ -24097,7 +24103,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C10" s="24" t="s">
         <v>17</v>
       </c>
@@ -24123,7 +24129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C11" s="24" t="s">
         <v>17</v>
       </c>
@@ -24148,14 +24154,14 @@
       <c r="J11" s="27">
         <v>20</v>
       </c>
-      <c r="M11" s="273" t="s">
-        <v>265</v>
-      </c>
-      <c r="N11" s="274">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M11" s="235" t="s">
+        <v>264</v>
+      </c>
+      <c r="N11" s="236">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
@@ -24181,7 +24187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C13" s="24" t="s">
         <v>17</v>
       </c>
@@ -24207,7 +24213,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C14" s="24" t="s">
         <v>17</v>
       </c>
@@ -24232,8 +24238,11 @@
       <c r="J14" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C15" s="24" t="s">
         <v>17</v>
       </c>
@@ -24268,7 +24277,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C16" s="24" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Final allocation exec - country and comp
</commit_message>
<xml_diff>
--- a/SDBal/input_data.xlsx
+++ b/SDBal/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\SDBal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30E0F65-2BBF-460D-9617-068398A8F698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F30E249-272A-4F97-9726-012861A930C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -923,7 +923,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2402" uniqueCount="267">
   <si>
     <t>Lot Size (MT)</t>
   </si>
@@ -1720,9 +1720,6 @@
   </si>
   <si>
     <t xml:space="preserve">Quantity to Trim: </t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>Customer level</t>
@@ -3898,76 +3895,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="87" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3994,6 +3922,9 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4001,6 +3932,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11847,7 +11844,7 @@
         <v>196</v>
       </c>
       <c r="P16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -20147,10 +20144,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="271" t="s">
+      <c r="D3" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="272"/>
+      <c r="E3" s="250"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -20263,11 +20260,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="239" t="s">
+      <c r="L14" s="260" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="239"/>
-      <c r="N14" s="239"/>
+      <c r="M14" s="260"/>
+      <c r="N14" s="260"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -20294,13 +20291,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="273" t="s">
+      <c r="F16" s="251" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="258" t="s">
+      <c r="G16" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="260" t="s">
+      <c r="H16" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -20324,9 +20321,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="273"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="248"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="255"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -20345,11 +20342,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="273"/>
-      <c r="G18" s="249" t="s">
+      <c r="F18" s="251"/>
+      <c r="G18" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="247" t="s">
+      <c r="H18" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -20372,9 +20369,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="273"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="248"/>
+      <c r="F19" s="251"/>
+      <c r="G19" s="253"/>
+      <c r="H19" s="255"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -20393,11 +20390,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="273"/>
-      <c r="G20" s="249" t="s">
+      <c r="F20" s="251"/>
+      <c r="G20" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="247" t="s">
+      <c r="H20" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -20421,9 +20418,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="273"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="248"/>
+      <c r="F21" s="251"/>
+      <c r="G21" s="253"/>
+      <c r="H21" s="255"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -20442,11 +20439,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="273"/>
-      <c r="G22" s="249" t="s">
+      <c r="F22" s="251"/>
+      <c r="G22" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="247" t="s">
+      <c r="H22" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -20470,9 +20467,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="273"/>
-      <c r="G23" s="250"/>
-      <c r="H23" s="251"/>
+      <c r="F23" s="251"/>
+      <c r="G23" s="258"/>
+      <c r="H23" s="259"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -20491,7 +20488,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="273"/>
+      <c r="F24" s="251"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -20536,11 +20533,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="261" t="s">
+      <c r="F26" s="239" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="261"/>
-      <c r="H26" s="261"/>
+      <c r="G26" s="239"/>
+      <c r="H26" s="239"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -20566,10 +20563,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="263" t="s">
+      <c r="G27" s="240" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="264"/>
+      <c r="H27" s="241"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -20593,8 +20590,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="265"/>
-      <c r="H28" s="266"/>
+      <c r="G28" s="242"/>
+      <c r="H28" s="243"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -20619,8 +20616,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="265"/>
-      <c r="H29" s="266"/>
+      <c r="G29" s="242"/>
+      <c r="H29" s="243"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -20639,8 +20636,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="265"/>
-      <c r="H30" s="266"/>
+      <c r="G30" s="242"/>
+      <c r="H30" s="243"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -20662,8 +20659,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="265"/>
-      <c r="H31" s="266"/>
+      <c r="G31" s="242"/>
+      <c r="H31" s="243"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -20685,8 +20682,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="267"/>
-      <c r="H32" s="268"/>
+      <c r="G32" s="244"/>
+      <c r="H32" s="245"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -20728,10 +20725,10 @@
       </c>
     </row>
     <row r="34" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="269" t="s">
+      <c r="G34" s="246" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="270"/>
+      <c r="H34" s="247"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -20753,8 +20750,8 @@
       </c>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G35" s="267"/>
-      <c r="H35" s="268"/>
+      <c r="G35" s="244"/>
+      <c r="H35" s="245"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -20855,11 +20852,11 @@
       </c>
     </row>
     <row r="40" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="261" t="s">
+      <c r="F40" s="239" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="261"/>
-      <c r="H40" s="262"/>
+      <c r="G40" s="239"/>
+      <c r="H40" s="248"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -20896,11 +20893,11 @@
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="261" t="s">
+      <c r="F42" s="239" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="261"/>
-      <c r="H42" s="262"/>
+      <c r="G42" s="239"/>
+      <c r="H42" s="248"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -20921,12 +20918,12 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="242" t="s">
+      <c r="E43" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="242"/>
-      <c r="G43" s="242"/>
-      <c r="H43" s="242"/>
+      <c r="F43" s="263"/>
+      <c r="G43" s="263"/>
+      <c r="H43" s="263"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -20950,11 +20947,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="243" t="s">
+      <c r="L44" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="244"/>
-      <c r="N44" s="253" t="s">
+      <c r="M44" s="265"/>
+      <c r="N44" s="269" t="s">
         <v>77</v>
       </c>
     </row>
@@ -20962,16 +20959,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="243"/>
-      <c r="M45" s="244"/>
-      <c r="N45" s="254"/>
+      <c r="L45" s="264"/>
+      <c r="M45" s="265"/>
+      <c r="N45" s="270"/>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="245"/>
-      <c r="M46" s="246"/>
+      <c r="L46" s="266"/>
+      <c r="M46" s="267"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.3">
@@ -21045,10 +21042,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="255" t="s">
+      <c r="M55" s="271" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="256"/>
+      <c r="N55" s="272"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -21075,13 +21072,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="257" t="s">
+      <c r="F57" s="273" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="258" t="s">
+      <c r="G57" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="260" t="s">
+      <c r="H57" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -21105,9 +21102,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="257"/>
-      <c r="G58" s="259"/>
-      <c r="H58" s="248"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="253"/>
+      <c r="H58" s="255"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -21129,11 +21126,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="257"/>
-      <c r="G59" s="249" t="s">
+      <c r="F59" s="273"/>
+      <c r="G59" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="247" t="s">
+      <c r="H59" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -21157,9 +21154,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="257"/>
-      <c r="G60" s="259"/>
-      <c r="H60" s="248"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="253"/>
+      <c r="H60" s="255"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -21181,11 +21178,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="257"/>
-      <c r="G61" s="249" t="s">
+      <c r="F61" s="273"/>
+      <c r="G61" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="247" t="s">
+      <c r="H61" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -21209,9 +21206,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="257"/>
-      <c r="G62" s="259"/>
-      <c r="H62" s="248"/>
+      <c r="F62" s="273"/>
+      <c r="G62" s="253"/>
+      <c r="H62" s="255"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -21233,11 +21230,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="257"/>
-      <c r="G63" s="249" t="s">
+      <c r="F63" s="273"/>
+      <c r="G63" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="247" t="s">
+      <c r="H63" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -21261,9 +21258,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="257"/>
-      <c r="G64" s="250"/>
-      <c r="H64" s="251"/>
+      <c r="F64" s="273"/>
+      <c r="G64" s="258"/>
+      <c r="H64" s="259"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -21348,10 +21345,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="252" t="s">
+      <c r="G68" s="268" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="252"/>
+      <c r="H68" s="268"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -21373,8 +21370,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="252"/>
-      <c r="H69" s="252"/>
+      <c r="G69" s="268"/>
+      <c r="H69" s="268"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -21399,8 +21396,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="252"/>
-      <c r="H70" s="252"/>
+      <c r="G70" s="268"/>
+      <c r="H70" s="268"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -21422,10 +21419,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="240" t="s">
+      <c r="G71" s="261" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="241"/>
+      <c r="H71" s="262"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -21447,10 +21444,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="252" t="s">
+      <c r="G72" s="268" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="252"/>
+      <c r="H72" s="268"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -21472,8 +21469,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="252"/>
-      <c r="H73" s="252"/>
+      <c r="G73" s="268"/>
+      <c r="H73" s="268"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -21498,8 +21495,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="252"/>
-      <c r="H74" s="252"/>
+      <c r="G74" s="268"/>
+      <c r="H74" s="268"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -21519,10 +21516,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="240" t="s">
+      <c r="G75" s="261" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="241"/>
+      <c r="H75" s="262"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -21565,12 +21562,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="242" t="s">
+      <c r="E77" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="242"/>
-      <c r="G77" s="242"/>
-      <c r="H77" s="242"/>
+      <c r="F77" s="263"/>
+      <c r="G77" s="263"/>
+      <c r="H77" s="263"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -21589,18 +21586,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="243" t="s">
+      <c r="L78" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="244"/>
+      <c r="M78" s="265"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="243"/>
-      <c r="M79" s="244"/>
+      <c r="L79" s="264"/>
+      <c r="M79" s="265"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="245"/>
-      <c r="M80" s="246"/>
+      <c r="L80" s="266"/>
+      <c r="M80" s="267"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -21694,25 +21691,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="G27:H32"/>
-    <mergeCell ref="G34:H35"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F42:H42"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="G75:H75"/>
     <mergeCell ref="E77:H77"/>
@@ -21729,6 +21707,25 @@
     <mergeCell ref="M55:N55"/>
     <mergeCell ref="F57:F64"/>
     <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="G27:H32"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21793,10 +21790,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="271" t="s">
+      <c r="D3" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="272"/>
+      <c r="E3" s="250"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -21912,10 +21909,10 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="255" t="s">
+      <c r="L14" s="271" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="256"/>
+      <c r="M14" s="272"/>
       <c r="N14" s="275"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21943,13 +21940,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="273" t="s">
+      <c r="F16" s="251" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="258" t="s">
+      <c r="G16" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="260" t="s">
+      <c r="H16" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -21973,9 +21970,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="273"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="248"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="255"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -21994,11 +21991,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="273"/>
-      <c r="G18" s="249" t="s">
+      <c r="F18" s="251"/>
+      <c r="G18" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="247" t="s">
+      <c r="H18" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -22022,9 +22019,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="273"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="248"/>
+      <c r="F19" s="251"/>
+      <c r="G19" s="253"/>
+      <c r="H19" s="255"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -22043,11 +22040,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="273"/>
-      <c r="G20" s="249" t="s">
+      <c r="F20" s="251"/>
+      <c r="G20" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="247" t="s">
+      <c r="H20" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -22071,9 +22068,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="273"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="248"/>
+      <c r="F21" s="251"/>
+      <c r="G21" s="253"/>
+      <c r="H21" s="255"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -22092,11 +22089,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="273"/>
-      <c r="G22" s="249" t="s">
+      <c r="F22" s="251"/>
+      <c r="G22" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="247" t="s">
+      <c r="H22" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -22120,9 +22117,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="273"/>
-      <c r="G23" s="250"/>
-      <c r="H23" s="251"/>
+      <c r="F23" s="251"/>
+      <c r="G23" s="258"/>
+      <c r="H23" s="259"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -22141,7 +22138,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="273"/>
+      <c r="F24" s="251"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -22184,11 +22181,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="261" t="s">
+      <c r="F26" s="239" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="261"/>
-      <c r="H26" s="261"/>
+      <c r="G26" s="239"/>
+      <c r="H26" s="239"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -22216,10 +22213,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="263" t="s">
+      <c r="G27" s="240" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="264"/>
+      <c r="H27" s="241"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -22244,8 +22241,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="265"/>
-      <c r="H28" s="266"/>
+      <c r="G28" s="242"/>
+      <c r="H28" s="243"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -22270,8 +22267,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="265"/>
-      <c r="H29" s="266"/>
+      <c r="G29" s="242"/>
+      <c r="H29" s="243"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -22290,8 +22287,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="265"/>
-      <c r="H30" s="266"/>
+      <c r="G30" s="242"/>
+      <c r="H30" s="243"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -22313,8 +22310,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="265"/>
-      <c r="H31" s="266"/>
+      <c r="G31" s="242"/>
+      <c r="H31" s="243"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -22336,8 +22333,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="267"/>
-      <c r="H32" s="268"/>
+      <c r="G32" s="244"/>
+      <c r="H32" s="245"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -22379,10 +22376,10 @@
       </c>
     </row>
     <row r="34" spans="5:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="269" t="s">
+      <c r="G34" s="246" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="270"/>
+      <c r="H34" s="247"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -22404,8 +22401,8 @@
       </c>
     </row>
     <row r="35" spans="5:21" x14ac:dyDescent="0.3">
-      <c r="G35" s="267"/>
-      <c r="H35" s="268"/>
+      <c r="G35" s="244"/>
+      <c r="H35" s="245"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -22506,11 +22503,11 @@
       </c>
     </row>
     <row r="40" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="261" t="s">
+      <c r="F40" s="239" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="261"/>
-      <c r="H40" s="262"/>
+      <c r="G40" s="239"/>
+      <c r="H40" s="248"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -22547,11 +22544,11 @@
       </c>
     </row>
     <row r="42" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="261" t="s">
+      <c r="F42" s="239" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="261"/>
-      <c r="H42" s="262"/>
+      <c r="G42" s="239"/>
+      <c r="H42" s="248"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -22572,12 +22569,12 @@
       </c>
     </row>
     <row r="43" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="242" t="s">
+      <c r="E43" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="242"/>
-      <c r="G43" s="242"/>
-      <c r="H43" s="242"/>
+      <c r="F43" s="263"/>
+      <c r="G43" s="263"/>
+      <c r="H43" s="263"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -22599,10 +22596,10 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="243" t="s">
+      <c r="L44" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="244"/>
+      <c r="M44" s="265"/>
       <c r="N44" s="274" t="s">
         <v>77</v>
       </c>
@@ -22611,16 +22608,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="243"/>
-      <c r="M45" s="244"/>
-      <c r="N45" s="254"/>
+      <c r="L45" s="264"/>
+      <c r="M45" s="265"/>
+      <c r="N45" s="270"/>
     </row>
     <row r="46" spans="5:21" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="245"/>
-      <c r="M46" s="246"/>
+      <c r="L46" s="266"/>
+      <c r="M46" s="267"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:21" x14ac:dyDescent="0.3">
@@ -22702,10 +22699,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="255" t="s">
+      <c r="M55" s="271" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="256"/>
+      <c r="N55" s="272"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -22732,13 +22729,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="257" t="s">
+      <c r="F57" s="273" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="258" t="s">
+      <c r="G57" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="260" t="s">
+      <c r="H57" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -22762,9 +22759,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="257"/>
-      <c r="G58" s="259"/>
-      <c r="H58" s="248"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="253"/>
+      <c r="H58" s="255"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -22786,11 +22783,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="257"/>
-      <c r="G59" s="249" t="s">
+      <c r="F59" s="273"/>
+      <c r="G59" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="247" t="s">
+      <c r="H59" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -22814,9 +22811,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="257"/>
-      <c r="G60" s="259"/>
-      <c r="H60" s="248"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="253"/>
+      <c r="H60" s="255"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -22838,11 +22835,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="257"/>
-      <c r="G61" s="249" t="s">
+      <c r="F61" s="273"/>
+      <c r="G61" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="247" t="s">
+      <c r="H61" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -22866,9 +22863,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="257"/>
-      <c r="G62" s="259"/>
-      <c r="H62" s="248"/>
+      <c r="F62" s="273"/>
+      <c r="G62" s="253"/>
+      <c r="H62" s="255"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -22890,11 +22887,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="257"/>
-      <c r="G63" s="249" t="s">
+      <c r="F63" s="273"/>
+      <c r="G63" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="247" t="s">
+      <c r="H63" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -22918,9 +22915,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="257"/>
-      <c r="G64" s="250"/>
-      <c r="H64" s="251"/>
+      <c r="F64" s="273"/>
+      <c r="G64" s="258"/>
+      <c r="H64" s="259"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -23005,10 +23002,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="252" t="s">
+      <c r="G68" s="268" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="252"/>
+      <c r="H68" s="268"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -23030,8 +23027,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="252"/>
-      <c r="H69" s="252"/>
+      <c r="G69" s="268"/>
+      <c r="H69" s="268"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -23056,8 +23053,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="252"/>
-      <c r="H70" s="252"/>
+      <c r="G70" s="268"/>
+      <c r="H70" s="268"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -23079,10 +23076,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="240" t="s">
+      <c r="G71" s="261" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="241"/>
+      <c r="H71" s="262"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -23104,10 +23101,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="252" t="s">
+      <c r="G72" s="268" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="252"/>
+      <c r="H72" s="268"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -23129,8 +23126,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="252"/>
-      <c r="H73" s="252"/>
+      <c r="G73" s="268"/>
+      <c r="H73" s="268"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -23155,8 +23152,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="252"/>
-      <c r="H74" s="252"/>
+      <c r="G74" s="268"/>
+      <c r="H74" s="268"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -23176,10 +23173,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="240" t="s">
+      <c r="G75" s="261" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="241"/>
+      <c r="H75" s="262"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -23222,12 +23219,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="242" t="s">
+      <c r="E77" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="242"/>
-      <c r="G77" s="242"/>
-      <c r="H77" s="242"/>
+      <c r="F77" s="263"/>
+      <c r="G77" s="263"/>
+      <c r="H77" s="263"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -23246,18 +23243,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="243" t="s">
+      <c r="L78" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="244"/>
+      <c r="M78" s="265"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="243"/>
-      <c r="M79" s="244"/>
+      <c r="L79" s="264"/>
+      <c r="M79" s="265"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="245"/>
-      <c r="M80" s="246"/>
+      <c r="L80" s="266"/>
+      <c r="M80" s="267"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -23345,25 +23342,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="N44:N45"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="L44:M46"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
     <mergeCell ref="L78:M80"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="F26:H26"/>
@@ -23380,6 +23358,25 @@
     <mergeCell ref="G57:G58"/>
     <mergeCell ref="H57:H58"/>
     <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="N44:N45"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="L44:M46"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="L14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23785,10 +23782,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA26EA1-65D7-4B0C-A5C0-83D8CE19816C}">
-  <dimension ref="C2:S86"/>
+  <dimension ref="C2:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23810,7 +23807,7 @@
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
@@ -23842,10 +23839,10 @@
         <v>261</v>
       </c>
       <c r="N2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="20" t="s">
         <v>17</v>
       </c>
@@ -23881,10 +23878,10 @@
         <v>22</v>
       </c>
       <c r="R3" s="231" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C4" s="24" t="s">
         <v>17</v>
       </c>
@@ -23923,7 +23920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C5" s="24" t="s">
         <v>17</v>
       </c>
@@ -23962,7 +23959,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C6" s="24" t="s">
         <v>17</v>
       </c>
@@ -24001,7 +23998,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="24" t="s">
         <v>17</v>
       </c>
@@ -24040,7 +24037,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C8" s="24" t="s">
         <v>17</v>
       </c>
@@ -24074,7 +24071,7 @@
       </c>
       <c r="R8" s="276"/>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C9" s="24" t="s">
         <v>17</v>
       </c>
@@ -24103,7 +24100,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C10" s="24" t="s">
         <v>17</v>
       </c>
@@ -24129,7 +24126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C11" s="24" t="s">
         <v>17</v>
       </c>
@@ -24158,10 +24155,10 @@
         <v>264</v>
       </c>
       <c r="N11" s="236">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
@@ -24187,7 +24184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C13" s="24" t="s">
         <v>17</v>
       </c>
@@ -24213,7 +24210,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C14" s="24" t="s">
         <v>17</v>
       </c>
@@ -24238,11 +24235,8 @@
       <c r="J14" s="27">
         <v>10</v>
       </c>
-      <c r="S14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C15" s="24" t="s">
         <v>17</v>
       </c>
@@ -24277,7 +24271,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C16" s="24" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Alter alloc to trim for country
</commit_message>
<xml_diff>
--- a/SDBal/input_data.xlsx
+++ b/SDBal/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\SDBal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F30E249-272A-4F97-9726-012861A930C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69E672C-93E8-4913-8CD1-6EF4DD0E7E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="1236" windowWidth="10500" windowHeight="10380" tabRatio="723" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rank_sept" sheetId="21" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3895,7 +3895,76 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="87" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3922,9 +3991,6 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3932,72 +3998,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8403,7 +8403,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
@@ -20144,10 +20144,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="249" t="s">
+      <c r="D3" s="271" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="250"/>
+      <c r="E3" s="272"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -20260,11 +20260,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="260" t="s">
+      <c r="L14" s="239" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="260"/>
-      <c r="N14" s="260"/>
+      <c r="M14" s="239"/>
+      <c r="N14" s="239"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -20291,13 +20291,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="251" t="s">
+      <c r="F16" s="273" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="252" t="s">
+      <c r="G16" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="254" t="s">
+      <c r="H16" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -20321,9 +20321,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="251"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="255"/>
+      <c r="F17" s="273"/>
+      <c r="G17" s="259"/>
+      <c r="H17" s="248"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -20342,11 +20342,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="251"/>
-      <c r="G18" s="256" t="s">
+      <c r="F18" s="273"/>
+      <c r="G18" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="257" t="s">
+      <c r="H18" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -20369,9 +20369,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="251"/>
-      <c r="G19" s="253"/>
-      <c r="H19" s="255"/>
+      <c r="F19" s="273"/>
+      <c r="G19" s="259"/>
+      <c r="H19" s="248"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -20390,11 +20390,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="251"/>
-      <c r="G20" s="256" t="s">
+      <c r="F20" s="273"/>
+      <c r="G20" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="257" t="s">
+      <c r="H20" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -20418,9 +20418,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="251"/>
-      <c r="G21" s="253"/>
-      <c r="H21" s="255"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="259"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -20439,11 +20439,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="251"/>
-      <c r="G22" s="256" t="s">
+      <c r="F22" s="273"/>
+      <c r="G22" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="257" t="s">
+      <c r="H22" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -20467,9 +20467,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="251"/>
-      <c r="G23" s="258"/>
-      <c r="H23" s="259"/>
+      <c r="F23" s="273"/>
+      <c r="G23" s="250"/>
+      <c r="H23" s="251"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -20488,7 +20488,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="251"/>
+      <c r="F24" s="273"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -20533,11 +20533,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="239" t="s">
+      <c r="F26" s="261" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="239"/>
-      <c r="H26" s="239"/>
+      <c r="G26" s="261"/>
+      <c r="H26" s="261"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -20563,10 +20563,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="240" t="s">
+      <c r="G27" s="263" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="241"/>
+      <c r="H27" s="264"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -20590,8 +20590,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="242"/>
-      <c r="H28" s="243"/>
+      <c r="G28" s="265"/>
+      <c r="H28" s="266"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -20616,8 +20616,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="242"/>
-      <c r="H29" s="243"/>
+      <c r="G29" s="265"/>
+      <c r="H29" s="266"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -20636,8 +20636,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="242"/>
-      <c r="H30" s="243"/>
+      <c r="G30" s="265"/>
+      <c r="H30" s="266"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -20659,8 +20659,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="242"/>
-      <c r="H31" s="243"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="266"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -20682,8 +20682,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="244"/>
-      <c r="H32" s="245"/>
+      <c r="G32" s="267"/>
+      <c r="H32" s="268"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -20725,10 +20725,10 @@
       </c>
     </row>
     <row r="34" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="246" t="s">
+      <c r="G34" s="269" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="247"/>
+      <c r="H34" s="270"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -20750,8 +20750,8 @@
       </c>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G35" s="244"/>
-      <c r="H35" s="245"/>
+      <c r="G35" s="267"/>
+      <c r="H35" s="268"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -20852,11 +20852,11 @@
       </c>
     </row>
     <row r="40" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="239" t="s">
+      <c r="F40" s="261" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="239"/>
-      <c r="H40" s="248"/>
+      <c r="G40" s="261"/>
+      <c r="H40" s="262"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -20893,11 +20893,11 @@
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="239" t="s">
+      <c r="F42" s="261" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="239"/>
-      <c r="H42" s="248"/>
+      <c r="G42" s="261"/>
+      <c r="H42" s="262"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -20918,12 +20918,12 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="263" t="s">
+      <c r="E43" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="263"/>
-      <c r="G43" s="263"/>
-      <c r="H43" s="263"/>
+      <c r="F43" s="242"/>
+      <c r="G43" s="242"/>
+      <c r="H43" s="242"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -20947,11 +20947,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="264" t="s">
+      <c r="L44" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="265"/>
-      <c r="N44" s="269" t="s">
+      <c r="M44" s="244"/>
+      <c r="N44" s="253" t="s">
         <v>77</v>
       </c>
     </row>
@@ -20959,16 +20959,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="264"/>
-      <c r="M45" s="265"/>
-      <c r="N45" s="270"/>
+      <c r="L45" s="243"/>
+      <c r="M45" s="244"/>
+      <c r="N45" s="254"/>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="266"/>
-      <c r="M46" s="267"/>
+      <c r="L46" s="245"/>
+      <c r="M46" s="246"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.3">
@@ -21042,10 +21042,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="271" t="s">
+      <c r="M55" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="272"/>
+      <c r="N55" s="256"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -21072,13 +21072,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="273" t="s">
+      <c r="F57" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="252" t="s">
+      <c r="G57" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="254" t="s">
+      <c r="H57" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -21102,9 +21102,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="273"/>
-      <c r="G58" s="253"/>
-      <c r="H58" s="255"/>
+      <c r="F58" s="257"/>
+      <c r="G58" s="259"/>
+      <c r="H58" s="248"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -21126,11 +21126,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="273"/>
-      <c r="G59" s="256" t="s">
+      <c r="F59" s="257"/>
+      <c r="G59" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="257" t="s">
+      <c r="H59" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -21154,9 +21154,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="273"/>
-      <c r="G60" s="253"/>
-      <c r="H60" s="255"/>
+      <c r="F60" s="257"/>
+      <c r="G60" s="259"/>
+      <c r="H60" s="248"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -21178,11 +21178,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="273"/>
-      <c r="G61" s="256" t="s">
+      <c r="F61" s="257"/>
+      <c r="G61" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="257" t="s">
+      <c r="H61" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -21206,9 +21206,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="273"/>
-      <c r="G62" s="253"/>
-      <c r="H62" s="255"/>
+      <c r="F62" s="257"/>
+      <c r="G62" s="259"/>
+      <c r="H62" s="248"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -21230,11 +21230,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="273"/>
-      <c r="G63" s="256" t="s">
+      <c r="F63" s="257"/>
+      <c r="G63" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="257" t="s">
+      <c r="H63" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -21258,9 +21258,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="273"/>
-      <c r="G64" s="258"/>
-      <c r="H64" s="259"/>
+      <c r="F64" s="257"/>
+      <c r="G64" s="250"/>
+      <c r="H64" s="251"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -21345,10 +21345,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="268" t="s">
+      <c r="G68" s="252" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="268"/>
+      <c r="H68" s="252"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -21370,8 +21370,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="268"/>
-      <c r="H69" s="268"/>
+      <c r="G69" s="252"/>
+      <c r="H69" s="252"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -21396,8 +21396,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="268"/>
-      <c r="H70" s="268"/>
+      <c r="G70" s="252"/>
+      <c r="H70" s="252"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -21419,10 +21419,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="261" t="s">
+      <c r="G71" s="240" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="262"/>
+      <c r="H71" s="241"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -21444,10 +21444,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="268" t="s">
+      <c r="G72" s="252" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="268"/>
+      <c r="H72" s="252"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -21469,8 +21469,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="268"/>
-      <c r="H73" s="268"/>
+      <c r="G73" s="252"/>
+      <c r="H73" s="252"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -21495,8 +21495,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="268"/>
-      <c r="H74" s="268"/>
+      <c r="G74" s="252"/>
+      <c r="H74" s="252"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -21516,10 +21516,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="261" t="s">
+      <c r="G75" s="240" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="262"/>
+      <c r="H75" s="241"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -21562,12 +21562,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="263" t="s">
+      <c r="E77" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="263"/>
-      <c r="G77" s="263"/>
-      <c r="H77" s="263"/>
+      <c r="F77" s="242"/>
+      <c r="G77" s="242"/>
+      <c r="H77" s="242"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -21586,18 +21586,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="264" t="s">
+      <c r="L78" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="265"/>
+      <c r="M78" s="244"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="264"/>
-      <c r="M79" s="265"/>
+      <c r="L79" s="243"/>
+      <c r="M79" s="244"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="266"/>
-      <c r="M80" s="267"/>
+      <c r="L80" s="245"/>
+      <c r="M80" s="246"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -21691,6 +21691,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="G27:H32"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F42:H42"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="G75:H75"/>
     <mergeCell ref="E77:H77"/>
@@ -21707,25 +21726,6 @@
     <mergeCell ref="M55:N55"/>
     <mergeCell ref="F57:F64"/>
     <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="G27:H32"/>
-    <mergeCell ref="G34:H35"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21790,10 +21790,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="249" t="s">
+      <c r="D3" s="271" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="250"/>
+      <c r="E3" s="272"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -21909,10 +21909,10 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="271" t="s">
+      <c r="L14" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="272"/>
+      <c r="M14" s="256"/>
       <c r="N14" s="275"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21940,13 +21940,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="251" t="s">
+      <c r="F16" s="273" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="252" t="s">
+      <c r="G16" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="254" t="s">
+      <c r="H16" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -21970,9 +21970,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="251"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="255"/>
+      <c r="F17" s="273"/>
+      <c r="G17" s="259"/>
+      <c r="H17" s="248"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -21991,11 +21991,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="251"/>
-      <c r="G18" s="256" t="s">
+      <c r="F18" s="273"/>
+      <c r="G18" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="257" t="s">
+      <c r="H18" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -22019,9 +22019,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="251"/>
-      <c r="G19" s="253"/>
-      <c r="H19" s="255"/>
+      <c r="F19" s="273"/>
+      <c r="G19" s="259"/>
+      <c r="H19" s="248"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -22040,11 +22040,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="251"/>
-      <c r="G20" s="256" t="s">
+      <c r="F20" s="273"/>
+      <c r="G20" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="257" t="s">
+      <c r="H20" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -22068,9 +22068,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="251"/>
-      <c r="G21" s="253"/>
-      <c r="H21" s="255"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="259"/>
+      <c r="H21" s="248"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -22089,11 +22089,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="251"/>
-      <c r="G22" s="256" t="s">
+      <c r="F22" s="273"/>
+      <c r="G22" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="257" t="s">
+      <c r="H22" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -22117,9 +22117,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="251"/>
-      <c r="G23" s="258"/>
-      <c r="H23" s="259"/>
+      <c r="F23" s="273"/>
+      <c r="G23" s="250"/>
+      <c r="H23" s="251"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -22138,7 +22138,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="251"/>
+      <c r="F24" s="273"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -22181,11 +22181,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="239" t="s">
+      <c r="F26" s="261" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="239"/>
-      <c r="H26" s="239"/>
+      <c r="G26" s="261"/>
+      <c r="H26" s="261"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -22213,10 +22213,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="240" t="s">
+      <c r="G27" s="263" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="241"/>
+      <c r="H27" s="264"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -22241,8 +22241,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="242"/>
-      <c r="H28" s="243"/>
+      <c r="G28" s="265"/>
+      <c r="H28" s="266"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -22267,8 +22267,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="242"/>
-      <c r="H29" s="243"/>
+      <c r="G29" s="265"/>
+      <c r="H29" s="266"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -22287,8 +22287,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="242"/>
-      <c r="H30" s="243"/>
+      <c r="G30" s="265"/>
+      <c r="H30" s="266"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -22310,8 +22310,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="242"/>
-      <c r="H31" s="243"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="266"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -22333,8 +22333,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="244"/>
-      <c r="H32" s="245"/>
+      <c r="G32" s="267"/>
+      <c r="H32" s="268"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -22376,10 +22376,10 @@
       </c>
     </row>
     <row r="34" spans="5:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="246" t="s">
+      <c r="G34" s="269" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="247"/>
+      <c r="H34" s="270"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -22401,8 +22401,8 @@
       </c>
     </row>
     <row r="35" spans="5:21" x14ac:dyDescent="0.3">
-      <c r="G35" s="244"/>
-      <c r="H35" s="245"/>
+      <c r="G35" s="267"/>
+      <c r="H35" s="268"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -22503,11 +22503,11 @@
       </c>
     </row>
     <row r="40" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="239" t="s">
+      <c r="F40" s="261" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="239"/>
-      <c r="H40" s="248"/>
+      <c r="G40" s="261"/>
+      <c r="H40" s="262"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -22544,11 +22544,11 @@
       </c>
     </row>
     <row r="42" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="239" t="s">
+      <c r="F42" s="261" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="239"/>
-      <c r="H42" s="248"/>
+      <c r="G42" s="261"/>
+      <c r="H42" s="262"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -22569,12 +22569,12 @@
       </c>
     </row>
     <row r="43" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="263" t="s">
+      <c r="E43" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="263"/>
-      <c r="G43" s="263"/>
-      <c r="H43" s="263"/>
+      <c r="F43" s="242"/>
+      <c r="G43" s="242"/>
+      <c r="H43" s="242"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -22596,10 +22596,10 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="264" t="s">
+      <c r="L44" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="265"/>
+      <c r="M44" s="244"/>
       <c r="N44" s="274" t="s">
         <v>77</v>
       </c>
@@ -22608,16 +22608,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="264"/>
-      <c r="M45" s="265"/>
-      <c r="N45" s="270"/>
+      <c r="L45" s="243"/>
+      <c r="M45" s="244"/>
+      <c r="N45" s="254"/>
     </row>
     <row r="46" spans="5:21" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="266"/>
-      <c r="M46" s="267"/>
+      <c r="L46" s="245"/>
+      <c r="M46" s="246"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:21" x14ac:dyDescent="0.3">
@@ -22699,10 +22699,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="271" t="s">
+      <c r="M55" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="272"/>
+      <c r="N55" s="256"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -22729,13 +22729,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="273" t="s">
+      <c r="F57" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="252" t="s">
+      <c r="G57" s="258" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="254" t="s">
+      <c r="H57" s="260" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -22759,9 +22759,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="273"/>
-      <c r="G58" s="253"/>
-      <c r="H58" s="255"/>
+      <c r="F58" s="257"/>
+      <c r="G58" s="259"/>
+      <c r="H58" s="248"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -22783,11 +22783,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="273"/>
-      <c r="G59" s="256" t="s">
+      <c r="F59" s="257"/>
+      <c r="G59" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="257" t="s">
+      <c r="H59" s="247" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -22811,9 +22811,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="273"/>
-      <c r="G60" s="253"/>
-      <c r="H60" s="255"/>
+      <c r="F60" s="257"/>
+      <c r="G60" s="259"/>
+      <c r="H60" s="248"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -22835,11 +22835,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="273"/>
-      <c r="G61" s="256" t="s">
+      <c r="F61" s="257"/>
+      <c r="G61" s="249" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="257" t="s">
+      <c r="H61" s="247" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -22863,9 +22863,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="273"/>
-      <c r="G62" s="253"/>
-      <c r="H62" s="255"/>
+      <c r="F62" s="257"/>
+      <c r="G62" s="259"/>
+      <c r="H62" s="248"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -22887,11 +22887,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="273"/>
-      <c r="G63" s="256" t="s">
+      <c r="F63" s="257"/>
+      <c r="G63" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="257" t="s">
+      <c r="H63" s="247" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -22915,9 +22915,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="273"/>
-      <c r="G64" s="258"/>
-      <c r="H64" s="259"/>
+      <c r="F64" s="257"/>
+      <c r="G64" s="250"/>
+      <c r="H64" s="251"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -23002,10 +23002,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="268" t="s">
+      <c r="G68" s="252" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="268"/>
+      <c r="H68" s="252"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -23027,8 +23027,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="268"/>
-      <c r="H69" s="268"/>
+      <c r="G69" s="252"/>
+      <c r="H69" s="252"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -23053,8 +23053,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="268"/>
-      <c r="H70" s="268"/>
+      <c r="G70" s="252"/>
+      <c r="H70" s="252"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -23076,10 +23076,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="261" t="s">
+      <c r="G71" s="240" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="262"/>
+      <c r="H71" s="241"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -23101,10 +23101,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="268" t="s">
+      <c r="G72" s="252" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="268"/>
+      <c r="H72" s="252"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -23126,8 +23126,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="268"/>
-      <c r="H73" s="268"/>
+      <c r="G73" s="252"/>
+      <c r="H73" s="252"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -23152,8 +23152,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="268"/>
-      <c r="H74" s="268"/>
+      <c r="G74" s="252"/>
+      <c r="H74" s="252"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -23173,10 +23173,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="261" t="s">
+      <c r="G75" s="240" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="262"/>
+      <c r="H75" s="241"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -23219,12 +23219,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="263" t="s">
+      <c r="E77" s="242" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="263"/>
-      <c r="G77" s="263"/>
-      <c r="H77" s="263"/>
+      <c r="F77" s="242"/>
+      <c r="G77" s="242"/>
+      <c r="H77" s="242"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -23243,18 +23243,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="264" t="s">
+      <c r="L78" s="243" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="265"/>
+      <c r="M78" s="244"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="264"/>
-      <c r="M79" s="265"/>
+      <c r="L79" s="243"/>
+      <c r="M79" s="244"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="266"/>
-      <c r="M80" s="267"/>
+      <c r="L80" s="245"/>
+      <c r="M80" s="246"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -23342,6 +23342,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="N44:N45"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="L44:M46"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
     <mergeCell ref="L78:M80"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="F26:H26"/>
@@ -23358,25 +23377,6 @@
     <mergeCell ref="G57:G58"/>
     <mergeCell ref="H57:H58"/>
     <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="N44:N45"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="L44:M46"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="L14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23784,8 +23784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA26EA1-65D7-4B0C-A5C0-83D8CE19816C}">
   <dimension ref="C2:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24155,7 +24155,7 @@
         <v>264</v>
       </c>
       <c r="N11" s="236">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Alter alloc_to_trim for customer done
</commit_message>
<xml_diff>
--- a/SDBal/input_data.xlsx
+++ b/SDBal/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\SDBal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69E672C-93E8-4913-8CD1-6EF4DD0E7E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111403EA-5C3E-4FC0-84DA-CC0976114E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="1236" windowWidth="10500" windowHeight="10380" tabRatio="723" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="1464" windowWidth="10500" windowHeight="10380" tabRatio="723" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rank_sept" sheetId="21" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3895,76 +3895,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="87" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3991,6 +3922,9 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="57" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3998,6 +3932,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="45" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="57" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="58" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="45" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8403,7 +8403,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8ECCA9-356C-4FF1-8BD5-D950D31C5068}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
@@ -20144,10 +20144,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="271" t="s">
+      <c r="D3" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="272"/>
+      <c r="E3" s="250"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -20260,11 +20260,11 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="239" t="s">
+      <c r="L14" s="260" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="239"/>
-      <c r="N14" s="239"/>
+      <c r="M14" s="260"/>
+      <c r="N14" s="260"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G15" s="56" t="s">
@@ -20291,13 +20291,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="273" t="s">
+      <c r="F16" s="251" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="258" t="s">
+      <c r="G16" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="260" t="s">
+      <c r="H16" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -20321,9 +20321,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="273"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="248"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="255"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -20342,11 +20342,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="273"/>
-      <c r="G18" s="249" t="s">
+      <c r="F18" s="251"/>
+      <c r="G18" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="247" t="s">
+      <c r="H18" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -20369,9 +20369,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="273"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="248"/>
+      <c r="F19" s="251"/>
+      <c r="G19" s="253"/>
+      <c r="H19" s="255"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -20390,11 +20390,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="273"/>
-      <c r="G20" s="249" t="s">
+      <c r="F20" s="251"/>
+      <c r="G20" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="247" t="s">
+      <c r="H20" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -20418,9 +20418,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="273"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="248"/>
+      <c r="F21" s="251"/>
+      <c r="G21" s="253"/>
+      <c r="H21" s="255"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -20439,11 +20439,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="273"/>
-      <c r="G22" s="249" t="s">
+      <c r="F22" s="251"/>
+      <c r="G22" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="247" t="s">
+      <c r="H22" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -20467,9 +20467,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="273"/>
-      <c r="G23" s="250"/>
-      <c r="H23" s="251"/>
+      <c r="F23" s="251"/>
+      <c r="G23" s="258"/>
+      <c r="H23" s="259"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -20488,7 +20488,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="273"/>
+      <c r="F24" s="251"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -20533,11 +20533,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="261" t="s">
+      <c r="F26" s="239" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="261"/>
-      <c r="H26" s="261"/>
+      <c r="G26" s="239"/>
+      <c r="H26" s="239"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -20563,10 +20563,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="263" t="s">
+      <c r="G27" s="240" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="264"/>
+      <c r="H27" s="241"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -20590,8 +20590,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="265"/>
-      <c r="H28" s="266"/>
+      <c r="G28" s="242"/>
+      <c r="H28" s="243"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -20616,8 +20616,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="265"/>
-      <c r="H29" s="266"/>
+      <c r="G29" s="242"/>
+      <c r="H29" s="243"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -20636,8 +20636,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="265"/>
-      <c r="H30" s="266"/>
+      <c r="G30" s="242"/>
+      <c r="H30" s="243"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -20659,8 +20659,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="265"/>
-      <c r="H31" s="266"/>
+      <c r="G31" s="242"/>
+      <c r="H31" s="243"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -20682,8 +20682,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="267"/>
-      <c r="H32" s="268"/>
+      <c r="G32" s="244"/>
+      <c r="H32" s="245"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -20725,10 +20725,10 @@
       </c>
     </row>
     <row r="34" spans="5:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="269" t="s">
+      <c r="G34" s="246" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="270"/>
+      <c r="H34" s="247"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -20750,8 +20750,8 @@
       </c>
     </row>
     <row r="35" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G35" s="267"/>
-      <c r="H35" s="268"/>
+      <c r="G35" s="244"/>
+      <c r="H35" s="245"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -20852,11 +20852,11 @@
       </c>
     </row>
     <row r="40" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="261" t="s">
+      <c r="F40" s="239" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="261"/>
-      <c r="H40" s="262"/>
+      <c r="G40" s="239"/>
+      <c r="H40" s="248"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -20893,11 +20893,11 @@
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="261" t="s">
+      <c r="F42" s="239" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="261"/>
-      <c r="H42" s="262"/>
+      <c r="G42" s="239"/>
+      <c r="H42" s="248"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -20918,12 +20918,12 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="242" t="s">
+      <c r="E43" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="242"/>
-      <c r="G43" s="242"/>
-      <c r="H43" s="242"/>
+      <c r="F43" s="263"/>
+      <c r="G43" s="263"/>
+      <c r="H43" s="263"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -20947,11 +20947,11 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="243" t="s">
+      <c r="L44" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="244"/>
-      <c r="N44" s="253" t="s">
+      <c r="M44" s="265"/>
+      <c r="N44" s="269" t="s">
         <v>77</v>
       </c>
     </row>
@@ -20959,16 +20959,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="243"/>
-      <c r="M45" s="244"/>
-      <c r="N45" s="254"/>
+      <c r="L45" s="264"/>
+      <c r="M45" s="265"/>
+      <c r="N45" s="270"/>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="245"/>
-      <c r="M46" s="246"/>
+      <c r="L46" s="266"/>
+      <c r="M46" s="267"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.3">
@@ -21042,10 +21042,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="255" t="s">
+      <c r="M55" s="271" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="256"/>
+      <c r="N55" s="272"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -21072,13 +21072,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="257" t="s">
+      <c r="F57" s="273" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="258" t="s">
+      <c r="G57" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="260" t="s">
+      <c r="H57" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -21102,9 +21102,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="257"/>
-      <c r="G58" s="259"/>
-      <c r="H58" s="248"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="253"/>
+      <c r="H58" s="255"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -21126,11 +21126,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="257"/>
-      <c r="G59" s="249" t="s">
+      <c r="F59" s="273"/>
+      <c r="G59" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="247" t="s">
+      <c r="H59" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -21154,9 +21154,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="257"/>
-      <c r="G60" s="259"/>
-      <c r="H60" s="248"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="253"/>
+      <c r="H60" s="255"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -21178,11 +21178,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="257"/>
-      <c r="G61" s="249" t="s">
+      <c r="F61" s="273"/>
+      <c r="G61" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="247" t="s">
+      <c r="H61" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -21206,9 +21206,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="257"/>
-      <c r="G62" s="259"/>
-      <c r="H62" s="248"/>
+      <c r="F62" s="273"/>
+      <c r="G62" s="253"/>
+      <c r="H62" s="255"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -21230,11 +21230,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="257"/>
-      <c r="G63" s="249" t="s">
+      <c r="F63" s="273"/>
+      <c r="G63" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="247" t="s">
+      <c r="H63" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -21258,9 +21258,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="257"/>
-      <c r="G64" s="250"/>
-      <c r="H64" s="251"/>
+      <c r="F64" s="273"/>
+      <c r="G64" s="258"/>
+      <c r="H64" s="259"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -21345,10 +21345,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="252" t="s">
+      <c r="G68" s="268" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="252"/>
+      <c r="H68" s="268"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -21370,8 +21370,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="252"/>
-      <c r="H69" s="252"/>
+      <c r="G69" s="268"/>
+      <c r="H69" s="268"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -21396,8 +21396,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="252"/>
-      <c r="H70" s="252"/>
+      <c r="G70" s="268"/>
+      <c r="H70" s="268"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -21419,10 +21419,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="240" t="s">
+      <c r="G71" s="261" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="241"/>
+      <c r="H71" s="262"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -21444,10 +21444,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="252" t="s">
+      <c r="G72" s="268" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="252"/>
+      <c r="H72" s="268"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -21469,8 +21469,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="252"/>
-      <c r="H73" s="252"/>
+      <c r="G73" s="268"/>
+      <c r="H73" s="268"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -21495,8 +21495,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="252"/>
-      <c r="H74" s="252"/>
+      <c r="G74" s="268"/>
+      <c r="H74" s="268"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -21516,10 +21516,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="240" t="s">
+      <c r="G75" s="261" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="241"/>
+      <c r="H75" s="262"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -21562,12 +21562,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="242" t="s">
+      <c r="E77" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="242"/>
-      <c r="G77" s="242"/>
-      <c r="H77" s="242"/>
+      <c r="F77" s="263"/>
+      <c r="G77" s="263"/>
+      <c r="H77" s="263"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -21586,18 +21586,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="243" t="s">
+      <c r="L78" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="244"/>
+      <c r="M78" s="265"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="243"/>
-      <c r="M79" s="244"/>
+      <c r="L79" s="264"/>
+      <c r="M79" s="265"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="245"/>
-      <c r="M80" s="246"/>
+      <c r="L80" s="266"/>
+      <c r="M80" s="267"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -21691,25 +21691,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="G27:H32"/>
-    <mergeCell ref="G34:H35"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F42:H42"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="G75:H75"/>
     <mergeCell ref="E77:H77"/>
@@ -21726,6 +21707,25 @@
     <mergeCell ref="M55:N55"/>
     <mergeCell ref="F57:F64"/>
     <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="G27:H32"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21790,10 +21790,10 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="271" t="s">
+      <c r="D3" s="249" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="272"/>
+      <c r="E3" s="250"/>
       <c r="G3" t="s">
         <v>53</v>
       </c>
@@ -21909,10 +21909,10 @@
       <c r="H13" s="66"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="255" t="s">
+      <c r="L14" s="271" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="256"/>
+      <c r="M14" s="272"/>
       <c r="N14" s="275"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21940,13 +21940,13 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="273" t="s">
+      <c r="F16" s="251" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="258" t="s">
+      <c r="G16" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="260" t="s">
+      <c r="H16" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="72" t="s">
@@ -21970,9 +21970,9 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="273"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="248"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="255"/>
       <c r="I17" s="70" t="s">
         <v>75</v>
       </c>
@@ -21991,11 +21991,11 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="273"/>
-      <c r="G18" s="249" t="s">
+      <c r="F18" s="251"/>
+      <c r="G18" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="247" t="s">
+      <c r="H18" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="73" t="s">
@@ -22019,9 +22019,9 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="273"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="248"/>
+      <c r="F19" s="251"/>
+      <c r="G19" s="253"/>
+      <c r="H19" s="255"/>
       <c r="I19" s="70" t="s">
         <v>75</v>
       </c>
@@ -22040,11 +22040,11 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="273"/>
-      <c r="G20" s="249" t="s">
+      <c r="F20" s="251"/>
+      <c r="G20" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="247" t="s">
+      <c r="H20" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="73" t="s">
@@ -22068,9 +22068,9 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="273"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="248"/>
+      <c r="F21" s="251"/>
+      <c r="G21" s="253"/>
+      <c r="H21" s="255"/>
       <c r="I21" s="70" t="s">
         <v>75</v>
       </c>
@@ -22089,11 +22089,11 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="273"/>
-      <c r="G22" s="249" t="s">
+      <c r="F22" s="251"/>
+      <c r="G22" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="247" t="s">
+      <c r="H22" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="73" t="s">
@@ -22117,9 +22117,9 @@
       </c>
     </row>
     <row r="23" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="273"/>
-      <c r="G23" s="250"/>
-      <c r="H23" s="251"/>
+      <c r="F23" s="251"/>
+      <c r="G23" s="258"/>
+      <c r="H23" s="259"/>
       <c r="I23" s="71" t="s">
         <v>75</v>
       </c>
@@ -22138,7 +22138,7 @@
       </c>
     </row>
     <row r="24" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F24" s="273"/>
+      <c r="F24" s="251"/>
       <c r="I24" s="47" t="s">
         <v>79</v>
       </c>
@@ -22181,11 +22181,11 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="261" t="s">
+      <c r="F26" s="239" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="261"/>
-      <c r="H26" s="261"/>
+      <c r="G26" s="239"/>
+      <c r="H26" s="239"/>
       <c r="I26" s="114" t="s">
         <v>51</v>
       </c>
@@ -22213,10 +22213,10 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="263" t="s">
+      <c r="G27" s="240" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="264"/>
+      <c r="H27" s="241"/>
       <c r="I27" s="6" t="s">
         <v>57</v>
       </c>
@@ -22241,8 +22241,8 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="265"/>
-      <c r="H28" s="266"/>
+      <c r="G28" s="242"/>
+      <c r="H28" s="243"/>
       <c r="I28" s="9" t="s">
         <v>56</v>
       </c>
@@ -22267,8 +22267,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="265"/>
-      <c r="H29" s="266"/>
+      <c r="G29" s="242"/>
+      <c r="H29" s="243"/>
       <c r="I29" s="9" t="s">
         <v>174</v>
       </c>
@@ -22287,8 +22287,8 @@
       </c>
     </row>
     <row r="30" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="265"/>
-      <c r="H30" s="266"/>
+      <c r="G30" s="242"/>
+      <c r="H30" s="243"/>
       <c r="I30" s="9" t="s">
         <v>140</v>
       </c>
@@ -22310,8 +22310,8 @@
       </c>
     </row>
     <row r="31" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G31" s="265"/>
-      <c r="H31" s="266"/>
+      <c r="G31" s="242"/>
+      <c r="H31" s="243"/>
       <c r="I31" s="9" t="s">
         <v>141</v>
       </c>
@@ -22333,8 +22333,8 @@
       </c>
     </row>
     <row r="32" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="267"/>
-      <c r="H32" s="268"/>
+      <c r="G32" s="244"/>
+      <c r="H32" s="245"/>
       <c r="I32" s="8" t="s">
         <v>71</v>
       </c>
@@ -22376,10 +22376,10 @@
       </c>
     </row>
     <row r="34" spans="5:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="269" t="s">
+      <c r="G34" s="246" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="270"/>
+      <c r="H34" s="247"/>
       <c r="I34" s="7" t="s">
         <v>57</v>
       </c>
@@ -22401,8 +22401,8 @@
       </c>
     </row>
     <row r="35" spans="5:21" x14ac:dyDescent="0.3">
-      <c r="G35" s="267"/>
-      <c r="H35" s="268"/>
+      <c r="G35" s="244"/>
+      <c r="H35" s="245"/>
       <c r="I35" s="127" t="s">
         <v>56</v>
       </c>
@@ -22503,11 +22503,11 @@
       </c>
     </row>
     <row r="40" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="261" t="s">
+      <c r="F40" s="239" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="261"/>
-      <c r="H40" s="262"/>
+      <c r="G40" s="239"/>
+      <c r="H40" s="248"/>
       <c r="I40" s="7" t="s">
         <v>80</v>
       </c>
@@ -22544,11 +22544,11 @@
       </c>
     </row>
     <row r="42" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="261" t="s">
+      <c r="F42" s="239" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="261"/>
-      <c r="H42" s="262"/>
+      <c r="G42" s="239"/>
+      <c r="H42" s="248"/>
       <c r="I42" s="65" t="s">
         <v>101</v>
       </c>
@@ -22569,12 +22569,12 @@
       </c>
     </row>
     <row r="43" spans="5:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="242" t="s">
+      <c r="E43" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="242"/>
-      <c r="G43" s="242"/>
-      <c r="H43" s="242"/>
+      <c r="F43" s="263"/>
+      <c r="G43" s="263"/>
+      <c r="H43" s="263"/>
       <c r="I43" s="96" t="s">
         <v>111</v>
       </c>
@@ -22596,10 +22596,10 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67"/>
-      <c r="L44" s="243" t="s">
+      <c r="L44" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M44" s="244"/>
+      <c r="M44" s="265"/>
       <c r="N44" s="274" t="s">
         <v>77</v>
       </c>
@@ -22608,16 +22608,16 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67"/>
-      <c r="L45" s="243"/>
-      <c r="M45" s="244"/>
-      <c r="N45" s="254"/>
+      <c r="L45" s="264"/>
+      <c r="M45" s="265"/>
+      <c r="N45" s="270"/>
     </row>
     <row r="46" spans="5:21" x14ac:dyDescent="0.3">
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67"/>
-      <c r="L46" s="245"/>
-      <c r="M46" s="246"/>
+      <c r="L46" s="266"/>
+      <c r="M46" s="267"/>
       <c r="N46" s="68"/>
     </row>
     <row r="47" spans="5:21" x14ac:dyDescent="0.3">
@@ -22699,10 +22699,10 @@
     </row>
     <row r="55" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1"/>
-      <c r="M55" s="255" t="s">
+      <c r="M55" s="271" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="256"/>
+      <c r="N55" s="272"/>
     </row>
     <row r="56" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G56" s="56" t="s">
@@ -22729,13 +22729,13 @@
       </c>
     </row>
     <row r="57" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="257" t="s">
+      <c r="F57" s="273" t="s">
         <v>52</v>
       </c>
-      <c r="G57" s="258" t="s">
+      <c r="G57" s="252" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="260" t="s">
+      <c r="H57" s="254" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="72" t="s">
@@ -22759,9 +22759,9 @@
       </c>
     </row>
     <row r="58" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="257"/>
-      <c r="G58" s="259"/>
-      <c r="H58" s="248"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="253"/>
+      <c r="H58" s="255"/>
       <c r="I58" s="70" t="s">
         <v>75</v>
       </c>
@@ -22783,11 +22783,11 @@
       </c>
     </row>
     <row r="59" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="257"/>
-      <c r="G59" s="249" t="s">
+      <c r="F59" s="273"/>
+      <c r="G59" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="247" t="s">
+      <c r="H59" s="257" t="s">
         <v>9</v>
       </c>
       <c r="I59" s="73" t="s">
@@ -22811,9 +22811,9 @@
       </c>
     </row>
     <row r="60" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F60" s="257"/>
-      <c r="G60" s="259"/>
-      <c r="H60" s="248"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="253"/>
+      <c r="H60" s="255"/>
       <c r="I60" s="70" t="s">
         <v>75</v>
       </c>
@@ -22835,11 +22835,11 @@
       </c>
     </row>
     <row r="61" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F61" s="257"/>
-      <c r="G61" s="249" t="s">
+      <c r="F61" s="273"/>
+      <c r="G61" s="256" t="s">
         <v>47</v>
       </c>
-      <c r="H61" s="247" t="s">
+      <c r="H61" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="73" t="s">
@@ -22863,9 +22863,9 @@
       </c>
     </row>
     <row r="62" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F62" s="257"/>
-      <c r="G62" s="259"/>
-      <c r="H62" s="248"/>
+      <c r="F62" s="273"/>
+      <c r="G62" s="253"/>
+      <c r="H62" s="255"/>
       <c r="I62" s="70" t="s">
         <v>75</v>
       </c>
@@ -22887,11 +22887,11 @@
       </c>
     </row>
     <row r="63" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F63" s="257"/>
-      <c r="G63" s="249" t="s">
+      <c r="F63" s="273"/>
+      <c r="G63" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="247" t="s">
+      <c r="H63" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -22915,9 +22915,9 @@
       </c>
     </row>
     <row r="64" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F64" s="257"/>
-      <c r="G64" s="250"/>
-      <c r="H64" s="251"/>
+      <c r="F64" s="273"/>
+      <c r="G64" s="258"/>
+      <c r="H64" s="259"/>
       <c r="I64" s="71" t="s">
         <v>75</v>
       </c>
@@ -23002,10 +23002,10 @@
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G68" s="252" t="s">
+      <c r="G68" s="268" t="s">
         <v>114</v>
       </c>
-      <c r="H68" s="252"/>
+      <c r="H68" s="268"/>
       <c r="I68" s="10" t="s">
         <v>57</v>
       </c>
@@ -23027,8 +23027,8 @@
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G69" s="252"/>
-      <c r="H69" s="252"/>
+      <c r="G69" s="268"/>
+      <c r="H69" s="268"/>
       <c r="I69" s="11" t="s">
         <v>56</v>
       </c>
@@ -23053,8 +23053,8 @@
       </c>
     </row>
     <row r="70" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="252"/>
-      <c r="H70" s="252"/>
+      <c r="G70" s="268"/>
+      <c r="H70" s="268"/>
       <c r="I70" s="11" t="s">
         <v>1</v>
       </c>
@@ -23076,10 +23076,10 @@
       </c>
     </row>
     <row r="71" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G71" s="240" t="s">
+      <c r="G71" s="261" t="s">
         <v>121</v>
       </c>
-      <c r="H71" s="241"/>
+      <c r="H71" s="262"/>
       <c r="I71" s="61" t="s">
         <v>51</v>
       </c>
@@ -23101,10 +23101,10 @@
       </c>
     </row>
     <row r="72" spans="5:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="252" t="s">
+      <c r="G72" s="268" t="s">
         <v>116</v>
       </c>
-      <c r="H72" s="252"/>
+      <c r="H72" s="268"/>
       <c r="I72" s="10" t="s">
         <v>57</v>
       </c>
@@ -23126,8 +23126,8 @@
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="G73" s="252"/>
-      <c r="H73" s="252"/>
+      <c r="G73" s="268"/>
+      <c r="H73" s="268"/>
       <c r="I73" s="11" t="s">
         <v>56</v>
       </c>
@@ -23152,8 +23152,8 @@
       </c>
     </row>
     <row r="74" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G74" s="252"/>
-      <c r="H74" s="252"/>
+      <c r="G74" s="268"/>
+      <c r="H74" s="268"/>
       <c r="I74" s="11" t="s">
         <v>1</v>
       </c>
@@ -23173,10 +23173,10 @@
       </c>
     </row>
     <row r="75" spans="5:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G75" s="240" t="s">
+      <c r="G75" s="261" t="s">
         <v>122</v>
       </c>
-      <c r="H75" s="241"/>
+      <c r="H75" s="262"/>
       <c r="I75" s="61" t="s">
         <v>51</v>
       </c>
@@ -23219,12 +23219,12 @@
       </c>
     </row>
     <row r="77" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E77" s="242" t="s">
+      <c r="E77" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="242"/>
-      <c r="G77" s="242"/>
-      <c r="H77" s="242"/>
+      <c r="F77" s="263"/>
+      <c r="G77" s="263"/>
+      <c r="H77" s="263"/>
       <c r="I77" s="96" t="s">
         <v>111</v>
       </c>
@@ -23243,18 +23243,18 @@
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L78" s="243" t="s">
+      <c r="L78" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="M78" s="244"/>
+      <c r="M78" s="265"/>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L79" s="243"/>
-      <c r="M79" s="244"/>
+      <c r="L79" s="264"/>
+      <c r="M79" s="265"/>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="L80" s="245"/>
-      <c r="M80" s="246"/>
+      <c r="L80" s="266"/>
+      <c r="M80" s="267"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
@@ -23342,25 +23342,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="N44:N45"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="L44:M46"/>
-    <mergeCell ref="F16:F24"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
     <mergeCell ref="L78:M80"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="F26:H26"/>
@@ -23377,6 +23358,25 @@
     <mergeCell ref="G57:G58"/>
     <mergeCell ref="H57:H58"/>
     <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="N44:N45"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="L44:M46"/>
+    <mergeCell ref="F16:F24"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="L14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23785,7 +23785,7 @@
   <dimension ref="C2:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23839,7 +23839,7 @@
         <v>261</v>
       </c>
       <c r="N2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -24155,7 +24155,7 @@
         <v>264</v>
       </c>
       <c r="N11" s="236">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.3">

</xml_diff>